<commit_message>
updating data for parkrun plot
</commit_message>
<xml_diff>
--- a/data/parkrunstats.xlsx
+++ b/data/parkrunstats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/parkrun-times/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiemillar/Documents/parkrun_times/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{386550F9-404D-DD45-AFE9-860906AE23A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0D928D5-3C7C-D84F-A39B-7CE9FDABF2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{75F32931-CFD6-8743-9F06-326BB481DB37}"/>
+    <workbookView xWindow="540" yWindow="920" windowWidth="14900" windowHeight="17360" xr2:uid="{75F32931-CFD6-8743-9F06-326BB481DB37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
   <si>
     <t>Sharpham Road Playing Fields</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:N152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,321 +558,321 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>45549</v>
+        <v>45654</v>
       </c>
       <c r="C2">
-        <v>21.58</v>
+        <v>22.14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
-        <v>45542</v>
+        <v>45651</v>
       </c>
       <c r="C3">
-        <v>22.52</v>
+        <v>22.09</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45647</v>
+      </c>
+      <c r="C4">
+        <v>21.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45640</v>
+      </c>
+      <c r="C5">
+        <v>20.420000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45633</v>
+      </c>
+      <c r="C6">
+        <v>21.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45626</v>
+      </c>
+      <c r="C7">
+        <v>21.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45619</v>
+      </c>
+      <c r="C8">
+        <v>23.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45612</v>
+      </c>
+      <c r="C9">
+        <v>21.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45605</v>
+      </c>
+      <c r="C10">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45598</v>
+      </c>
+      <c r="C11">
+        <v>21.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45591</v>
+      </c>
+      <c r="C12">
+        <v>21.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45584</v>
+      </c>
+      <c r="C13">
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45577</v>
+      </c>
+      <c r="C14">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45570</v>
+      </c>
+      <c r="C15">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45563</v>
+      </c>
+      <c r="C16">
+        <v>20.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45556</v>
+      </c>
+      <c r="C17">
+        <v>21.31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C18">
+        <v>21.58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45542</v>
+      </c>
+      <c r="C19">
+        <v>22.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B20" s="1">
         <v>45535</v>
       </c>
-      <c r="C4">
+      <c r="C20">
         <v>23.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6">
-        <v>45528</v>
-      </c>
-      <c r="C5">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>45521</v>
-      </c>
-      <c r="C6">
-        <v>22.58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6">
-        <v>45514</v>
-      </c>
-      <c r="C7">
-        <v>24.49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6">
-        <v>45507</v>
-      </c>
-      <c r="C8">
-        <v>27.14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45500</v>
-      </c>
-      <c r="C9">
-        <v>24.38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45493</v>
-      </c>
-      <c r="C10">
-        <v>26.58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6">
-        <v>45486</v>
-      </c>
-      <c r="C11">
-        <v>23.45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45479</v>
-      </c>
-      <c r="C12">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45472</v>
-      </c>
-      <c r="C13">
-        <v>26.06</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6">
-        <v>45465</v>
-      </c>
-      <c r="C14">
-        <v>36.26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C15">
-        <v>24.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="6">
-        <v>45451</v>
-      </c>
-      <c r="C16">
-        <v>24.55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="6">
-        <v>45444</v>
-      </c>
-      <c r="C17">
-        <v>25.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="6">
-        <v>45437</v>
-      </c>
-      <c r="C18">
-        <v>25.55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="6">
-        <v>45430</v>
-      </c>
-      <c r="C19">
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="6">
-        <v>45423</v>
-      </c>
-      <c r="C20">
-        <v>25.31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B21" s="6">
-        <v>45416</v>
+        <v>45528</v>
       </c>
       <c r="C21">
-        <v>25.57</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="6">
-        <v>45409</v>
+        <v>45521</v>
       </c>
       <c r="C22">
-        <v>25.29</v>
+        <v>22.58</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B23" s="6">
-        <v>45402</v>
+        <v>45514</v>
       </c>
       <c r="C23">
-        <v>25.36</v>
+        <v>24.49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B24" s="6">
-        <v>45395</v>
+        <v>45507</v>
       </c>
       <c r="C24">
-        <v>25.51</v>
+        <v>27.14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B25" s="6">
-        <v>45388</v>
+        <v>45500</v>
       </c>
       <c r="C25">
-        <v>26.04</v>
+        <v>24.38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" s="6">
-        <v>45381</v>
+        <v>45493</v>
       </c>
       <c r="C26">
-        <v>24.49</v>
+        <v>26.58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B27" s="6">
-        <v>45374</v>
+        <v>45486</v>
       </c>
       <c r="C27">
-        <v>24.21</v>
+        <v>23.45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28" s="6">
-        <v>45367</v>
+        <v>45479</v>
       </c>
       <c r="C28">
-        <v>25.38</v>
+        <v>25.44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B29" s="6">
-        <v>45360</v>
+        <v>45472</v>
       </c>
       <c r="C29">
-        <v>26.2</v>
+        <v>26.06</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B30" s="6">
-        <v>45353</v>
+        <v>45465</v>
       </c>
       <c r="C30">
-        <v>27.41</v>
+        <v>36.26</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,32 +880,32 @@
         <v>2</v>
       </c>
       <c r="B31" s="6">
-        <v>45346</v>
+        <v>45458</v>
       </c>
       <c r="C31">
-        <v>25.14</v>
+        <v>24.56</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B32" s="6">
-        <v>45339</v>
+        <v>45451</v>
       </c>
       <c r="C32">
-        <v>25.47</v>
+        <v>24.55</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B33" s="6">
-        <v>45332</v>
+        <v>45444</v>
       </c>
       <c r="C33">
-        <v>27.23</v>
+        <v>25.08</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -913,43 +913,43 @@
         <v>3</v>
       </c>
       <c r="B34" s="6">
-        <v>45325</v>
+        <v>45437</v>
       </c>
       <c r="C34">
-        <v>25.38</v>
+        <v>25.55</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B35" s="6">
-        <v>45318</v>
+        <v>45430</v>
       </c>
       <c r="C35">
-        <v>26.15</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" s="6">
-        <v>45311</v>
+        <v>45423</v>
       </c>
       <c r="C36">
-        <v>25.27</v>
+        <v>25.31</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37" s="6">
-        <v>45304</v>
+        <v>45416</v>
       </c>
       <c r="C37">
-        <v>24.39</v>
+        <v>25.57</v>
       </c>
       <c r="J37" s="1"/>
       <c r="M37" s="2"/>
@@ -957,13 +957,13 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B38" s="6">
-        <v>45297</v>
+        <v>45409</v>
       </c>
       <c r="C38">
-        <v>28</v>
+        <v>25.29</v>
       </c>
       <c r="J38" s="1"/>
       <c r="M38" s="2"/>
@@ -971,13 +971,13 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B39" s="6">
-        <v>45290</v>
+        <v>45402</v>
       </c>
       <c r="C39">
-        <v>26.32</v>
+        <v>25.36</v>
       </c>
       <c r="J39" s="1"/>
       <c r="M39" s="4"/>
@@ -985,13 +985,13 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B40" s="6">
-        <v>45283</v>
+        <v>45395</v>
       </c>
       <c r="C40">
-        <v>26.07</v>
+        <v>25.51</v>
       </c>
       <c r="J40" s="1"/>
       <c r="M40" s="4"/>
@@ -999,13 +999,13 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B41" s="6">
-        <v>45276</v>
+        <v>45388</v>
       </c>
       <c r="C41">
-        <v>27.07</v>
+        <v>26.04</v>
       </c>
       <c r="J41" s="1"/>
       <c r="M41" s="4"/>
@@ -1013,13 +1013,13 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B42" s="6">
-        <v>45269</v>
+        <v>45381</v>
       </c>
       <c r="C42">
-        <v>25.56</v>
+        <v>24.49</v>
       </c>
       <c r="J42" s="1"/>
       <c r="M42" s="4"/>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B43" s="6">
-        <v>45262</v>
+        <v>45374</v>
       </c>
       <c r="C43">
-        <v>26.48</v>
+        <v>24.21</v>
       </c>
       <c r="J43" s="1"/>
       <c r="M43" s="2"/>
@@ -1041,13 +1041,13 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B44" s="6">
-        <v>45255</v>
+        <v>45367</v>
       </c>
       <c r="C44">
-        <v>27.26</v>
+        <v>25.38</v>
       </c>
       <c r="J44" s="1"/>
       <c r="M44" s="4"/>
@@ -1055,13 +1055,13 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B45" s="6">
-        <v>45248</v>
+        <v>45360</v>
       </c>
       <c r="C45">
-        <v>28.25</v>
+        <v>26.2</v>
       </c>
       <c r="J45" s="1"/>
       <c r="M45" s="4"/>
@@ -1069,13 +1069,13 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B46" s="6">
-        <v>45241</v>
+        <v>45353</v>
       </c>
       <c r="C46">
-        <v>26.25</v>
+        <v>27.41</v>
       </c>
       <c r="J46" s="1"/>
       <c r="M46" s="4"/>
@@ -1083,13 +1083,13 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B47" s="6">
-        <v>45234</v>
+        <v>45346</v>
       </c>
       <c r="C47">
-        <v>26.13</v>
+        <v>25.14</v>
       </c>
       <c r="J47" s="1"/>
       <c r="M47" s="4"/>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B48" s="6">
-        <v>45227</v>
+        <v>45339</v>
       </c>
       <c r="C48">
-        <v>26.42</v>
+        <v>25.47</v>
       </c>
       <c r="J48" s="1"/>
       <c r="M48" s="4"/>
@@ -1111,13 +1111,13 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B49" s="6">
-        <v>45220</v>
+        <v>45332</v>
       </c>
       <c r="C49">
-        <v>25.34</v>
+        <v>27.23</v>
       </c>
       <c r="J49" s="1"/>
       <c r="M49" s="4"/>
@@ -1125,13 +1125,13 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B50" s="6">
-        <v>45213</v>
+        <v>45325</v>
       </c>
       <c r="C50">
-        <v>25.09</v>
+        <v>25.38</v>
       </c>
       <c r="J50" s="1"/>
       <c r="M50" s="4"/>
@@ -1139,13 +1139,13 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B51" s="6">
-        <v>45206</v>
+        <v>45318</v>
       </c>
       <c r="C51">
-        <v>25.34</v>
+        <v>26.15</v>
       </c>
       <c r="J51" s="1"/>
       <c r="M51" s="4"/>
@@ -1153,13 +1153,13 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B52" s="6">
-        <v>45199</v>
+        <v>45311</v>
       </c>
       <c r="C52">
-        <v>30.37</v>
+        <v>25.27</v>
       </c>
       <c r="J52" s="1"/>
       <c r="M52" s="4"/>
@@ -1167,13 +1167,13 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B53" s="6">
-        <v>45192</v>
+        <v>45304</v>
       </c>
       <c r="C53">
-        <v>25.09</v>
+        <v>24.39</v>
       </c>
       <c r="J53" s="1"/>
       <c r="M53" s="4"/>
@@ -1181,13 +1181,13 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B54" s="6">
-        <v>45185</v>
+        <v>45297</v>
       </c>
       <c r="C54">
-        <v>27.09</v>
+        <v>28</v>
       </c>
       <c r="J54" s="1"/>
       <c r="M54" s="4"/>
@@ -1195,13 +1195,13 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B55" s="6">
-        <v>45178</v>
+        <v>45290</v>
       </c>
       <c r="C55">
-        <v>26.49</v>
+        <v>26.32</v>
       </c>
       <c r="J55" s="1"/>
       <c r="M55" s="4"/>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B56" s="6">
-        <v>45171</v>
+        <v>45283</v>
       </c>
       <c r="C56">
-        <v>28.17</v>
+        <v>26.07</v>
       </c>
       <c r="J56" s="1"/>
       <c r="M56" s="4"/>
@@ -1223,13 +1223,13 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B57" s="6">
-        <v>45164</v>
+        <v>45276</v>
       </c>
       <c r="C57">
-        <v>25.56</v>
+        <v>27.07</v>
       </c>
       <c r="J57" s="1"/>
       <c r="M57" s="4"/>
@@ -1237,13 +1237,13 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B58" s="6">
-        <v>45157</v>
+        <v>45269</v>
       </c>
       <c r="C58">
-        <v>26.54</v>
+        <v>25.56</v>
       </c>
       <c r="J58" s="1"/>
       <c r="M58" s="4"/>
@@ -1251,13 +1251,13 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B59" s="6">
-        <v>45150</v>
+        <v>45262</v>
       </c>
       <c r="C59">
-        <v>27.42</v>
+        <v>26.48</v>
       </c>
       <c r="J59" s="1"/>
       <c r="M59" s="4"/>
@@ -1265,13 +1265,13 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B60" s="6">
-        <v>45143</v>
+        <v>45255</v>
       </c>
       <c r="C60">
-        <v>27.02</v>
+        <v>27.26</v>
       </c>
       <c r="J60" s="1"/>
       <c r="M60" s="4"/>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B61" s="6">
-        <v>45136</v>
+        <v>45248</v>
       </c>
       <c r="C61">
         <v>28.25</v>
@@ -1293,13 +1293,13 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B62" s="6">
-        <v>45129</v>
+        <v>45241</v>
       </c>
       <c r="C62">
-        <v>28.37</v>
+        <v>26.25</v>
       </c>
       <c r="J62" s="1"/>
       <c r="M62" s="4"/>
@@ -1307,13 +1307,13 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B63" s="6">
-        <v>45115</v>
+        <v>45234</v>
       </c>
       <c r="C63">
-        <v>27.04</v>
+        <v>26.13</v>
       </c>
       <c r="J63" s="1"/>
       <c r="M63" s="4"/>
@@ -1321,13 +1321,13 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B64" s="6">
-        <v>45108</v>
+        <v>45227</v>
       </c>
       <c r="C64">
-        <v>27.29</v>
+        <v>26.42</v>
       </c>
       <c r="J64" s="1"/>
       <c r="M64" s="4"/>
@@ -1335,13 +1335,13 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B65" s="6">
-        <v>45101</v>
+        <v>45220</v>
       </c>
       <c r="C65">
-        <v>29.15</v>
+        <v>25.34</v>
       </c>
       <c r="J65" s="1"/>
       <c r="M65" s="4"/>
@@ -1349,13 +1349,13 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B66" s="6">
-        <v>45094</v>
+        <v>45213</v>
       </c>
       <c r="C66">
-        <v>28.59</v>
+        <v>25.09</v>
       </c>
       <c r="J66" s="1"/>
       <c r="M66" s="4"/>
@@ -1366,10 +1366,10 @@
         <v>3</v>
       </c>
       <c r="B67" s="6">
-        <v>45087</v>
+        <v>45206</v>
       </c>
       <c r="C67">
-        <v>29.41</v>
+        <v>25.34</v>
       </c>
       <c r="J67" s="1"/>
       <c r="M67" s="4"/>
@@ -1377,13 +1377,13 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B68" s="6">
-        <v>45080</v>
+        <v>45199</v>
       </c>
       <c r="C68">
-        <v>28.07</v>
+        <v>30.37</v>
       </c>
       <c r="J68" s="1"/>
       <c r="M68" s="4"/>
@@ -1391,13 +1391,13 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B69" s="6">
-        <v>45073</v>
+        <v>45192</v>
       </c>
       <c r="C69">
-        <v>27.33</v>
+        <v>25.09</v>
       </c>
       <c r="J69" s="1"/>
       <c r="M69" s="4"/>
@@ -1405,13 +1405,13 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B70" s="6">
-        <v>45066</v>
+        <v>45185</v>
       </c>
       <c r="C70">
-        <v>28.09</v>
+        <v>27.09</v>
       </c>
       <c r="J70" s="1"/>
       <c r="M70" s="4"/>
@@ -1419,13 +1419,13 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B71" s="6">
-        <v>45059</v>
+        <v>45178</v>
       </c>
       <c r="C71">
-        <v>27.3</v>
+        <v>26.49</v>
       </c>
       <c r="J71" s="1"/>
       <c r="M71" s="4"/>
@@ -1433,13 +1433,13 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B72" s="6">
-        <v>45052</v>
+        <v>45171</v>
       </c>
       <c r="C72">
-        <v>27.59</v>
+        <v>28.17</v>
       </c>
       <c r="J72" s="1"/>
       <c r="M72" s="4"/>
@@ -1447,13 +1447,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B73" s="6">
-        <v>45045</v>
+        <v>45164</v>
       </c>
       <c r="C73">
-        <v>28.14</v>
+        <v>25.56</v>
       </c>
       <c r="J73" s="1"/>
       <c r="M73" s="4"/>
@@ -1461,13 +1461,13 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B74" s="6">
-        <v>45038</v>
+        <v>45157</v>
       </c>
       <c r="C74">
-        <v>27.25</v>
+        <v>26.54</v>
       </c>
       <c r="J74" s="1"/>
       <c r="M74" s="4"/>
@@ -1475,13 +1475,13 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B75" s="6">
-        <v>45031</v>
+        <v>45150</v>
       </c>
       <c r="C75">
-        <v>28.28</v>
+        <v>27.42</v>
       </c>
       <c r="J75" s="1"/>
       <c r="M75" s="4"/>
@@ -1489,13 +1489,13 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B76" s="6">
-        <v>45024</v>
+        <v>45143</v>
       </c>
       <c r="C76">
-        <v>28.53</v>
+        <v>27.02</v>
       </c>
       <c r="J76" s="1"/>
       <c r="M76" s="4"/>
@@ -1503,13 +1503,13 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B77" s="6">
-        <v>45017</v>
+        <v>45136</v>
       </c>
       <c r="C77">
-        <v>30.19</v>
+        <v>28.25</v>
       </c>
       <c r="J77" s="1"/>
       <c r="M77" s="4"/>
@@ -1517,13 +1517,13 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B78" s="6">
-        <v>45010</v>
+        <v>45129</v>
       </c>
       <c r="C78">
-        <v>29.45</v>
+        <v>28.37</v>
       </c>
       <c r="J78" s="1"/>
       <c r="M78" s="4"/>
@@ -1531,13 +1531,13 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B79" s="6">
-        <v>45003</v>
+        <v>45115</v>
       </c>
       <c r="C79">
-        <v>29.21</v>
+        <v>27.04</v>
       </c>
       <c r="J79" s="1"/>
       <c r="M79" s="4"/>
@@ -1548,10 +1548,10 @@
         <v>3</v>
       </c>
       <c r="B80" s="6">
-        <v>44996</v>
+        <v>45108</v>
       </c>
       <c r="C80">
-        <v>29.14</v>
+        <v>27.29</v>
       </c>
       <c r="J80" s="1"/>
       <c r="M80" s="4"/>
@@ -1562,10 +1562,10 @@
         <v>3</v>
       </c>
       <c r="B81" s="6">
-        <v>44989</v>
+        <v>45101</v>
       </c>
       <c r="C81">
-        <v>30.02</v>
+        <v>29.15</v>
       </c>
       <c r="J81" s="1"/>
       <c r="M81" s="4"/>
@@ -1573,13 +1573,13 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B82" s="6">
-        <v>44982</v>
+        <v>45094</v>
       </c>
       <c r="C82">
-        <v>32.380000000000003</v>
+        <v>28.59</v>
       </c>
       <c r="J82" s="1"/>
       <c r="M82" s="4"/>
@@ -1590,10 +1590,10 @@
         <v>3</v>
       </c>
       <c r="B83" s="6">
-        <v>44975</v>
+        <v>45087</v>
       </c>
       <c r="C83">
-        <v>30.17</v>
+        <v>29.41</v>
       </c>
       <c r="J83" s="1"/>
       <c r="M83" s="4"/>
@@ -1604,10 +1604,10 @@
         <v>3</v>
       </c>
       <c r="B84" s="6">
-        <v>44968</v>
+        <v>45080</v>
       </c>
       <c r="C84">
-        <v>30.54</v>
+        <v>28.07</v>
       </c>
       <c r="J84" s="1"/>
       <c r="M84" s="4"/>
@@ -1618,10 +1618,10 @@
         <v>3</v>
       </c>
       <c r="B85" s="6">
-        <v>44961</v>
+        <v>45073</v>
       </c>
       <c r="C85">
-        <v>31.15</v>
+        <v>27.33</v>
       </c>
       <c r="J85" s="1"/>
       <c r="M85" s="4"/>
@@ -1632,10 +1632,10 @@
         <v>3</v>
       </c>
       <c r="B86" s="6">
-        <v>44954</v>
+        <v>45066</v>
       </c>
       <c r="C86">
-        <v>30.2</v>
+        <v>28.09</v>
       </c>
       <c r="J86" s="1"/>
       <c r="M86" s="4"/>
@@ -1646,10 +1646,10 @@
         <v>3</v>
       </c>
       <c r="B87" s="6">
-        <v>44947</v>
+        <v>45059</v>
       </c>
       <c r="C87">
-        <v>29.35</v>
+        <v>27.3</v>
       </c>
       <c r="J87" s="1"/>
       <c r="M87" s="4"/>
@@ -1660,10 +1660,10 @@
         <v>3</v>
       </c>
       <c r="B88" s="6">
-        <v>44940</v>
+        <v>45052</v>
       </c>
       <c r="C88">
-        <v>30.35</v>
+        <v>27.59</v>
       </c>
       <c r="J88" s="1"/>
       <c r="M88" s="4"/>
@@ -1674,10 +1674,10 @@
         <v>3</v>
       </c>
       <c r="B89" s="6">
-        <v>44933</v>
+        <v>45045</v>
       </c>
       <c r="C89">
-        <v>32.18</v>
+        <v>28.14</v>
       </c>
       <c r="J89" s="1"/>
       <c r="M89" s="4"/>
@@ -1685,13 +1685,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B90" s="6">
-        <v>44926</v>
+        <v>45038</v>
       </c>
       <c r="C90">
-        <v>31.54</v>
+        <v>27.25</v>
       </c>
       <c r="J90" s="1"/>
       <c r="M90" s="4"/>
@@ -1699,13 +1699,13 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B91" s="6">
-        <v>44919</v>
+        <v>45031</v>
       </c>
       <c r="C91">
-        <v>30.04</v>
+        <v>28.28</v>
       </c>
       <c r="J91" s="1"/>
       <c r="M91" s="4"/>
@@ -1716,10 +1716,10 @@
         <v>3</v>
       </c>
       <c r="B92" s="6">
-        <v>44905</v>
+        <v>45024</v>
       </c>
       <c r="C92">
-        <v>33.020000000000003</v>
+        <v>28.53</v>
       </c>
       <c r="J92" s="1"/>
       <c r="M92" s="4"/>
@@ -1730,10 +1730,10 @@
         <v>3</v>
       </c>
       <c r="B93" s="6">
-        <v>44898</v>
+        <v>45017</v>
       </c>
       <c r="C93">
-        <v>31.38</v>
+        <v>30.19</v>
       </c>
       <c r="J93" s="1"/>
       <c r="M93" s="4"/>
@@ -1744,10 +1744,10 @@
         <v>3</v>
       </c>
       <c r="B94" s="6">
-        <v>44891</v>
+        <v>45010</v>
       </c>
       <c r="C94">
-        <v>31.55</v>
+        <v>29.45</v>
       </c>
       <c r="J94" s="1"/>
       <c r="M94" s="4"/>
@@ -1758,10 +1758,10 @@
         <v>3</v>
       </c>
       <c r="B95" s="6">
-        <v>44884</v>
+        <v>45003</v>
       </c>
       <c r="C95">
-        <v>31.29</v>
+        <v>29.21</v>
       </c>
       <c r="J95" s="1"/>
       <c r="M95" s="4"/>
@@ -1772,10 +1772,10 @@
         <v>3</v>
       </c>
       <c r="B96" s="6">
-        <v>44877</v>
+        <v>44996</v>
       </c>
       <c r="C96">
-        <v>31.34</v>
+        <v>29.14</v>
       </c>
       <c r="J96" s="1"/>
       <c r="M96" s="4"/>
@@ -1786,10 +1786,10 @@
         <v>3</v>
       </c>
       <c r="B97" s="6">
-        <v>44870</v>
+        <v>44989</v>
       </c>
       <c r="C97">
-        <v>30.58</v>
+        <v>30.02</v>
       </c>
       <c r="J97" s="1"/>
       <c r="M97" s="4"/>
@@ -1800,10 +1800,10 @@
         <v>3</v>
       </c>
       <c r="B98" s="6">
-        <v>44863</v>
+        <v>44982</v>
       </c>
       <c r="C98">
-        <v>31.15</v>
+        <v>32.380000000000003</v>
       </c>
       <c r="J98" s="1"/>
       <c r="M98" s="4"/>
@@ -1814,10 +1814,10 @@
         <v>3</v>
       </c>
       <c r="B99" s="6">
-        <v>44856</v>
+        <v>44975</v>
       </c>
       <c r="C99">
-        <v>31.36</v>
+        <v>30.17</v>
       </c>
       <c r="J99" s="1"/>
       <c r="M99" s="4"/>
@@ -1828,10 +1828,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="6">
-        <v>44849</v>
+        <v>44968</v>
       </c>
       <c r="C100">
-        <v>31.38</v>
+        <v>30.54</v>
       </c>
       <c r="J100" s="1"/>
       <c r="M100" s="4"/>
@@ -1842,10 +1842,10 @@
         <v>3</v>
       </c>
       <c r="B101" s="6">
-        <v>44842</v>
+        <v>44961</v>
       </c>
       <c r="C101">
-        <v>29.44</v>
+        <v>31.15</v>
       </c>
       <c r="J101" s="1"/>
       <c r="M101" s="4"/>
@@ -1856,10 +1856,10 @@
         <v>3</v>
       </c>
       <c r="B102" s="6">
-        <v>44835</v>
+        <v>44954</v>
       </c>
       <c r="C102">
-        <v>30.47</v>
+        <v>30.2</v>
       </c>
       <c r="J102" s="1"/>
       <c r="M102" s="4"/>
@@ -1870,10 +1870,10 @@
         <v>3</v>
       </c>
       <c r="B103" s="6">
-        <v>44828</v>
+        <v>44947</v>
       </c>
       <c r="C103">
-        <v>30.57</v>
+        <v>29.35</v>
       </c>
       <c r="J103" s="1"/>
       <c r="M103" s="4"/>
@@ -1884,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="B104" s="6">
-        <v>44821</v>
+        <v>44940</v>
       </c>
       <c r="C104">
-        <v>30.57</v>
+        <v>30.35</v>
       </c>
       <c r="J104" s="1"/>
       <c r="M104" s="4"/>
@@ -1898,10 +1898,10 @@
         <v>3</v>
       </c>
       <c r="B105" s="6">
-        <v>44814</v>
+        <v>44933</v>
       </c>
       <c r="C105">
-        <v>31.16</v>
+        <v>32.18</v>
       </c>
       <c r="J105" s="1"/>
       <c r="M105" s="4"/>
@@ -1909,13 +1909,13 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B106" s="6">
-        <v>44807</v>
+        <v>44926</v>
       </c>
       <c r="C106">
-        <v>32.19</v>
+        <v>31.54</v>
       </c>
       <c r="J106" s="1"/>
       <c r="M106" s="4"/>
@@ -1923,13 +1923,13 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B107" s="6">
-        <v>44800</v>
+        <v>44919</v>
       </c>
       <c r="C107">
-        <v>32.08</v>
+        <v>30.04</v>
       </c>
       <c r="J107" s="1"/>
       <c r="M107" s="4"/>
@@ -1940,10 +1940,10 @@
         <v>3</v>
       </c>
       <c r="B108" s="6">
-        <v>44793</v>
+        <v>44905</v>
       </c>
       <c r="C108">
-        <v>32.31</v>
+        <v>33.020000000000003</v>
       </c>
       <c r="J108" s="1"/>
       <c r="M108" s="4"/>
@@ -1954,10 +1954,10 @@
         <v>3</v>
       </c>
       <c r="B109" s="6">
-        <v>44779</v>
+        <v>44898</v>
       </c>
       <c r="C109">
-        <v>31.48</v>
+        <v>31.38</v>
       </c>
       <c r="J109" s="1"/>
       <c r="M109" s="4"/>
@@ -1968,10 +1968,10 @@
         <v>3</v>
       </c>
       <c r="B110" s="6">
-        <v>44772</v>
+        <v>44891</v>
       </c>
       <c r="C110">
-        <v>32.22</v>
+        <v>31.55</v>
       </c>
       <c r="J110" s="1"/>
       <c r="M110" s="4"/>
@@ -1982,10 +1982,10 @@
         <v>3</v>
       </c>
       <c r="B111" s="6">
-        <v>44730</v>
+        <v>44884</v>
       </c>
       <c r="C111">
-        <v>32.04</v>
+        <v>31.29</v>
       </c>
       <c r="J111" s="1"/>
       <c r="M111" s="4"/>
@@ -1996,10 +1996,10 @@
         <v>3</v>
       </c>
       <c r="B112" s="6">
-        <v>44723</v>
+        <v>44877</v>
       </c>
       <c r="C112">
-        <v>32.22</v>
+        <v>31.34</v>
       </c>
       <c r="J112" s="1"/>
       <c r="M112" s="4"/>
@@ -2010,10 +2010,10 @@
         <v>3</v>
       </c>
       <c r="B113" s="6">
-        <v>44716</v>
+        <v>44870</v>
       </c>
       <c r="C113">
-        <v>31.36</v>
+        <v>30.58</v>
       </c>
       <c r="J113" s="1"/>
       <c r="M113" s="4"/>
@@ -2024,10 +2024,10 @@
         <v>3</v>
       </c>
       <c r="B114" s="6">
-        <v>44709</v>
+        <v>44863</v>
       </c>
       <c r="C114">
-        <v>31.06</v>
+        <v>31.15</v>
       </c>
       <c r="J114" s="1"/>
       <c r="M114" s="4"/>
@@ -2038,10 +2038,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="6">
-        <v>44702</v>
+        <v>44856</v>
       </c>
       <c r="C115">
-        <v>31.12</v>
+        <v>31.36</v>
       </c>
       <c r="J115" s="1"/>
       <c r="M115" s="4"/>
@@ -2052,10 +2052,10 @@
         <v>3</v>
       </c>
       <c r="B116" s="6">
-        <v>44597</v>
+        <v>44849</v>
       </c>
       <c r="C116">
-        <v>31.4</v>
+        <v>31.38</v>
       </c>
       <c r="J116" s="1"/>
       <c r="M116" s="4"/>
@@ -2066,10 +2066,10 @@
         <v>3</v>
       </c>
       <c r="B117" s="6">
-        <v>44590</v>
+        <v>44842</v>
       </c>
       <c r="C117">
-        <v>33.28</v>
+        <v>29.44</v>
       </c>
       <c r="J117" s="1"/>
       <c r="M117" s="4"/>
@@ -2080,10 +2080,10 @@
         <v>3</v>
       </c>
       <c r="B118" s="6">
-        <v>44583</v>
+        <v>44835</v>
       </c>
       <c r="C118">
-        <v>32.32</v>
+        <v>30.47</v>
       </c>
       <c r="J118" s="1"/>
       <c r="M118" s="4"/>
@@ -2094,10 +2094,10 @@
         <v>3</v>
       </c>
       <c r="B119" s="6">
-        <v>44478</v>
+        <v>44828</v>
       </c>
       <c r="C119">
-        <v>34.08</v>
+        <v>30.57</v>
       </c>
       <c r="J119" s="1"/>
       <c r="M119" s="4"/>
@@ -2108,131 +2108,275 @@
         <v>3</v>
       </c>
       <c r="B120" s="6">
-        <v>44471</v>
+        <v>44821</v>
       </c>
       <c r="C120">
-        <v>35.5</v>
+        <v>30.57</v>
       </c>
       <c r="J120" s="1"/>
       <c r="M120" s="4"/>
       <c r="N120" s="3"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121" s="6">
+        <v>44814</v>
+      </c>
+      <c r="C121">
+        <v>31.16</v>
+      </c>
       <c r="J121" s="1"/>
       <c r="M121" s="4"/>
       <c r="N121" s="3"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" s="6">
+        <v>44807</v>
+      </c>
+      <c r="C122">
+        <v>32.19</v>
+      </c>
       <c r="J122" s="1"/>
       <c r="M122" s="4"/>
       <c r="N122" s="3"/>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" s="6">
+        <v>44800</v>
+      </c>
+      <c r="C123">
+        <v>32.08</v>
+      </c>
       <c r="J123" s="1"/>
       <c r="M123" s="4"/>
       <c r="N123" s="3"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" s="6">
+        <v>44793</v>
+      </c>
+      <c r="C124">
+        <v>32.31</v>
+      </c>
       <c r="J124" s="1"/>
       <c r="M124" s="4"/>
       <c r="N124" s="3"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" s="6">
+        <v>44779</v>
+      </c>
+      <c r="C125">
+        <v>31.48</v>
+      </c>
       <c r="J125" s="1"/>
       <c r="M125" s="4"/>
       <c r="N125" s="3"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" s="6">
+        <v>44772</v>
+      </c>
+      <c r="C126">
+        <v>32.22</v>
+      </c>
       <c r="J126" s="1"/>
       <c r="M126" s="4"/>
       <c r="N126" s="3"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127" s="6">
+        <v>44730</v>
+      </c>
+      <c r="C127">
+        <v>32.04</v>
+      </c>
       <c r="J127" s="1"/>
       <c r="M127" s="4"/>
       <c r="N127" s="3"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="6">
+        <v>44723</v>
+      </c>
+      <c r="C128">
+        <v>32.22</v>
+      </c>
       <c r="J128" s="1"/>
       <c r="M128" s="4"/>
       <c r="N128" s="3"/>
     </row>
-    <row r="129" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="6">
+        <v>44716</v>
+      </c>
+      <c r="C129">
+        <v>31.36</v>
+      </c>
       <c r="J129" s="1"/>
       <c r="M129" s="4"/>
       <c r="N129" s="3"/>
     </row>
-    <row r="130" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" s="6">
+        <v>44709</v>
+      </c>
+      <c r="C130">
+        <v>31.06</v>
+      </c>
       <c r="J130" s="1"/>
       <c r="M130" s="4"/>
       <c r="N130" s="3"/>
     </row>
-    <row r="131" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131" s="6">
+        <v>44702</v>
+      </c>
+      <c r="C131">
+        <v>31.12</v>
+      </c>
       <c r="J131" s="1"/>
       <c r="M131" s="4"/>
       <c r="N131" s="3"/>
     </row>
-    <row r="132" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" s="6">
+        <v>44597</v>
+      </c>
+      <c r="C132">
+        <v>31.4</v>
+      </c>
       <c r="J132" s="1"/>
       <c r="M132" s="4"/>
       <c r="N132" s="3"/>
     </row>
-    <row r="133" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" s="6">
+        <v>44590</v>
+      </c>
+      <c r="C133">
+        <v>33.28</v>
+      </c>
       <c r="J133" s="1"/>
       <c r="M133" s="4"/>
       <c r="N133" s="3"/>
     </row>
-    <row r="134" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" s="6">
+        <v>44583</v>
+      </c>
+      <c r="C134">
+        <v>32.32</v>
+      </c>
       <c r="J134" s="1"/>
       <c r="M134" s="4"/>
       <c r="N134" s="3"/>
     </row>
-    <row r="135" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" s="6">
+        <v>44478</v>
+      </c>
+      <c r="C135">
+        <v>34.08</v>
+      </c>
       <c r="J135" s="1"/>
       <c r="M135" s="4"/>
       <c r="N135" s="3"/>
     </row>
-    <row r="136" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" s="6">
+        <v>44471</v>
+      </c>
+      <c r="C136">
+        <v>35.5</v>
+      </c>
       <c r="J136" s="1"/>
       <c r="M136" s="4"/>
       <c r="N136" s="3"/>
     </row>
-    <row r="137" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J137" s="1"/>
       <c r="M137" s="4"/>
       <c r="N137" s="3"/>
     </row>
-    <row r="138" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J138" s="1"/>
       <c r="M138" s="4"/>
       <c r="N138" s="3"/>
     </row>
-    <row r="139" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J139" s="1"/>
       <c r="M139" s="4"/>
       <c r="N139" s="3"/>
     </row>
-    <row r="140" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J140" s="1"/>
       <c r="M140" s="4"/>
       <c r="N140" s="3"/>
     </row>
-    <row r="141" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J141" s="1"/>
       <c r="M141" s="4"/>
       <c r="N141" s="3"/>
     </row>
-    <row r="142" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J142" s="1"/>
       <c r="M142" s="4"/>
       <c r="N142" s="3"/>
     </row>
-    <row r="143" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J143" s="1"/>
       <c r="M143" s="4"/>
       <c r="N143" s="3"/>
     </row>
-    <row r="144" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J144" s="1"/>
       <c r="M144" s="4"/>
       <c r="N144" s="3"/>
@@ -2279,238 +2423,238 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/" xr:uid="{252F5143-8A22-9B42-AF19-A38C76AD6802}"/>
-    <hyperlink ref="A6" r:id="rId2" display="https://www.parkrun.org.uk/lancingbeachgreen/results/" xr:uid="{150F9A52-4040-DA4A-85D2-D42805046243}"/>
-    <hyperlink ref="A7" r:id="rId3" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{BA78F95F-3373-604E-9550-F9E9EF53853F}"/>
-    <hyperlink ref="A8" r:id="rId4" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{40DFFB7F-349A-3149-B170-0BBC7FA11376}"/>
-    <hyperlink ref="A9" r:id="rId5" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{AA4429C8-98C4-3547-BFC6-C557606F2095}"/>
-    <hyperlink ref="A10" r:id="rId6" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B59B6240-6A79-F840-B20F-17478D063E0C}"/>
-    <hyperlink ref="A11" r:id="rId7" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{A6747A4E-8473-ED4B-A863-3C1462B63A87}"/>
-    <hyperlink ref="A12" r:id="rId8" display="https://www.parkrun.org.uk/catton/results/" xr:uid="{E3235270-25A9-9742-AC78-C6FB78EB746A}"/>
-    <hyperlink ref="A13" r:id="rId9" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3308C1A0-1C47-0C45-AD10-E078B08E84FC}"/>
-    <hyperlink ref="A14" r:id="rId10" display="https://www.parkrun.org.uk/greatyarmouthnorthbeach/results/" xr:uid="{E2A8AE47-AEA1-E44E-A199-19E11D7701DB}"/>
-    <hyperlink ref="A15" r:id="rId11" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{D9F72049-A833-0843-8159-D44B0C17A0F2}"/>
-    <hyperlink ref="A16" r:id="rId12" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6CA9A3C6-9033-2D44-B763-080A52A3718E}"/>
-    <hyperlink ref="A17" r:id="rId13" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B948A7B6-701C-874F-AD10-52310D121ECF}"/>
-    <hyperlink ref="A18" r:id="rId14" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{5F6095C9-2D81-2041-AF22-39BB4B6E1FA1}"/>
-    <hyperlink ref="A19" r:id="rId15" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{20872887-70C5-8049-B79C-D77851A224BE}"/>
-    <hyperlink ref="A20" r:id="rId16" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{61B7BAE3-6120-C244-933B-74AFEB167CB2}"/>
-    <hyperlink ref="A21" r:id="rId17" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{77B35723-636C-414F-8CEA-21D73264A764}"/>
-    <hyperlink ref="A22" r:id="rId18" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{504E6E96-07D3-C940-972F-02BCFE77CD66}"/>
-    <hyperlink ref="A23" r:id="rId19" display="https://www.parkrun.org.uk/swaffham/results/" xr:uid="{F7E130F9-71A3-034A-BCD8-9C5433C3D2F2}"/>
-    <hyperlink ref="A24" r:id="rId20" display="https://www.parkrun.org.uk/lowestoft/results/" xr:uid="{CBBA3CCB-DE8F-FA4C-876C-F56FD93D48FE}"/>
-    <hyperlink ref="A25" r:id="rId21" display="https://www.parkrun.org.uk/gorleston/results/" xr:uid="{D19FD83E-B7F7-634D-B167-462C567C2D4C}"/>
-    <hyperlink ref="A26" r:id="rId22" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{8519BDAB-3B2D-E944-8BE3-918E6C2F0EC5}"/>
-    <hyperlink ref="A27" r:id="rId23" display="https://www.parkrun.org.uk/gorleston/results/" xr:uid="{98AAA3A6-E767-3645-8D46-91EDBE0F0041}"/>
-    <hyperlink ref="A28" r:id="rId24" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{FDC42F18-28C5-9544-9F4E-861278ECB8EC}"/>
-    <hyperlink ref="A29" r:id="rId25" display="https://www.parkrun.org.uk/sandringham/results/" xr:uid="{925F3C71-F640-9543-AA11-78FDAE8F1988}"/>
-    <hyperlink ref="A30" r:id="rId26" display="https://www.parkrun.org.uk/brandoncountrypark/results/" xr:uid="{E77E37E4-D552-014F-95E9-94839E4DC9E7}"/>
-    <hyperlink ref="A31" r:id="rId27" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{E67019B4-05BA-9C48-9D0B-4D7996ACADDE}"/>
-    <hyperlink ref="A32" r:id="rId28" display="https://www.parkrun.org.uk/downhammarketacademy/results/" xr:uid="{4B14F13C-9004-8E49-9644-330FC85E3187}"/>
-    <hyperlink ref="A33" r:id="rId29" display="https://www.parkrun.org.uk/holkham/results/" xr:uid="{D1D42CE4-1B9D-A347-A668-27648D573172}"/>
-    <hyperlink ref="A34" r:id="rId30" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{F7EFF658-EC1C-7B4E-92FD-5F07789417A2}"/>
-    <hyperlink ref="A35" r:id="rId31" display="https://www.parkrun.org.uk/harlestonmagpies/results/" xr:uid="{5A43BF3F-61E2-084B-A1EB-AA9F3FE90FA2}"/>
-    <hyperlink ref="A36" r:id="rId32" display="https://www.parkrun.org.uk/catton/results/" xr:uid="{DE7DFFB6-7932-3D44-B06E-9FF86D65E128}"/>
-    <hyperlink ref="A37" r:id="rId33" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{D36393C6-CDF1-B541-919C-20BB8B44A055}"/>
-    <hyperlink ref="A38" r:id="rId34" display="https://www.parkrun.org.uk/altonwater/results/" xr:uid="{B49D816D-65CD-6345-AF36-8F5D2D6F2DD2}"/>
-    <hyperlink ref="A39" r:id="rId35" display="https://www.parkrun.org.uk/fivearches/results/" xr:uid="{DF90DA80-328B-1F4E-AD0D-451881682315}"/>
-    <hyperlink ref="A40" r:id="rId36" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/" xr:uid="{D67D01BA-A614-BC47-A357-5DEE330A639A}"/>
-    <hyperlink ref="A41" r:id="rId37" display="https://www.parkrun.org.uk/kingslynn/results/" xr:uid="{9B3D9FAB-2F2B-F04D-B98B-86A237E8BEFE}"/>
-    <hyperlink ref="A42" r:id="rId38" display="https://www.parkrun.org.uk/thetford/results/" xr:uid="{0173A15B-333E-5A4A-89FF-CFAF8CB0A408}"/>
-    <hyperlink ref="A43" r:id="rId39" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{845864C9-A5AA-FB4E-B257-7EAD70D2A84F}"/>
-    <hyperlink ref="A44" r:id="rId40" display="https://www.parkrun.org.uk/sheringham/results/" xr:uid="{365454C0-82CB-3F4F-8C1E-9C3A3998F3C0}"/>
-    <hyperlink ref="A45" r:id="rId41" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2E6F02C3-E788-8F44-99AB-6C806F37B49C}"/>
-    <hyperlink ref="A46" r:id="rId42" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{038CCF2F-9AE8-254D-8881-FDF710086E84}"/>
-    <hyperlink ref="A47" r:id="rId43" display="https://www.parkrun.org.uk/flegghigh/results/" xr:uid="{56BC7901-47C2-3145-8BBB-FFF3DE713576}"/>
-    <hyperlink ref="A48" r:id="rId44" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{4FC66B5F-2CE0-2247-A578-3992703E9896}"/>
-    <hyperlink ref="A49" r:id="rId45" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{5E398874-BF44-4344-9D7C-3C99BAFDB2A8}"/>
-    <hyperlink ref="A50" r:id="rId46" display="https://www.parkrun.org.uk/blickling/results/" xr:uid="{801E4171-29D4-EF4B-8E64-4A363FEC37C1}"/>
-    <hyperlink ref="A51" r:id="rId47" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{1467205D-F890-3C4F-833C-5F20EAA517A1}"/>
-    <hyperlink ref="A52" r:id="rId48" display="https://www.parkrun.org.uk/lochneaton/results/" xr:uid="{E33089F3-68BD-1E44-A176-6BCC42EBD3D5}"/>
-    <hyperlink ref="A53" r:id="rId49" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{380AB618-03F9-A94F-9D0A-E87743178E6B}"/>
-    <hyperlink ref="A54" r:id="rId50" display="https://www.parkrun.org.uk/northwalsham/results/" xr:uid="{BD0A4B75-0054-F844-A891-406B46E42F7B}"/>
-    <hyperlink ref="A55" r:id="rId51" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{16ECAEF5-D501-214E-BB0B-AD9526B41263}"/>
-    <hyperlink ref="A56" r:id="rId52" display="https://www.parkrun.org.uk/thornhamwalks/results/" xr:uid="{30AF7899-6690-5D4C-89D6-AD2ADB364F33}"/>
-    <hyperlink ref="A57" r:id="rId53" display="https://www.parkrun.org.uk/ifieldmillpond/results/" xr:uid="{0F571825-498D-AC4A-A040-E5834134979F}"/>
-    <hyperlink ref="A58" r:id="rId54" display="https://www.parkrun.org.uk/lingwood/results/" xr:uid="{764330BE-DC68-2E4E-8734-7D93450DFB66}"/>
-    <hyperlink ref="A59" r:id="rId55" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{CA96D4E5-6490-B848-A17A-FF069DC8604A}"/>
-    <hyperlink ref="A60" r:id="rId56" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{D0C1E86A-C330-DB40-BAA0-77264FCE0C23}"/>
-    <hyperlink ref="A61" r:id="rId57" display="https://www.parkrun.org.uk/street/results/" xr:uid="{F3B8A3FF-6369-AF41-BE95-9530C386002F}"/>
-    <hyperlink ref="A62" r:id="rId58" display="https://www.parkrun.org.uk/street/results/" xr:uid="{8CCE05DF-2116-3A42-A504-4DFAFC3EB05D}"/>
-    <hyperlink ref="A63" r:id="rId59" display="https://www.parkrun.org.uk/street/results/" xr:uid="{4E54B80E-A3E6-104B-9375-403534648F81}"/>
-    <hyperlink ref="A64" r:id="rId60" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{48C5576D-0058-2E48-9CC2-C287C64176C0}"/>
-    <hyperlink ref="A65" r:id="rId61" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{65B5A2BE-625A-C344-82F9-CC7E7572E2C8}"/>
-    <hyperlink ref="A66" r:id="rId62" display="https://www.parkrun.org.uk/brundall/results/" xr:uid="{F1B54B20-A89D-4746-975A-93D721F6B098}"/>
-    <hyperlink ref="A67" r:id="rId63" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A817D26B-6260-4D43-8B48-C501D9B554DA}"/>
-    <hyperlink ref="A68" r:id="rId64" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{8FEB1C36-5771-254F-A34B-81B6E0B0E92B}"/>
-    <hyperlink ref="A69" r:id="rId65" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{07BE9A8E-E930-314E-88B5-6B403477CC9B}"/>
-    <hyperlink ref="A70" r:id="rId66" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{86F146B6-D354-8049-A03B-C534E7126A50}"/>
-    <hyperlink ref="A71" r:id="rId67" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{1AF8CE9C-E6F3-BC49-A37C-703F79801090}"/>
-    <hyperlink ref="A72" r:id="rId68" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{537CF7E1-771F-F140-90CA-167E905B8DB7}"/>
-    <hyperlink ref="A73" r:id="rId69" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{9DB1979F-9A6F-6846-9E9B-15C948E6086E}"/>
-    <hyperlink ref="A74" r:id="rId70" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{94DCDC74-0483-914F-AE56-14F015F17617}"/>
-    <hyperlink ref="A75" r:id="rId71" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{98BFC344-5F98-2142-BF8B-BB64DC5DC176}"/>
-    <hyperlink ref="A76" r:id="rId72" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{152159AF-1135-ED49-A618-642813444F0B}"/>
-    <hyperlink ref="A77" r:id="rId73" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{782991EE-775E-1546-AC50-21A63A97DED3}"/>
-    <hyperlink ref="A78" r:id="rId74" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3AA8F00C-5402-EE44-812C-82FD37A2D123}"/>
-    <hyperlink ref="A79" r:id="rId75" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A620B43D-EFB5-7248-BED3-BB4F86A9B6CE}"/>
-    <hyperlink ref="A80" r:id="rId76" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{705246F0-97DB-F14C-8CBE-C6F161F61999}"/>
-    <hyperlink ref="A81" r:id="rId77" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{C9B996B1-3496-1B41-8B36-E0C135D5852E}"/>
-    <hyperlink ref="A82" r:id="rId78" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B3F85754-A195-B04D-AA5B-9CA78330AF14}"/>
-    <hyperlink ref="A83" r:id="rId79" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E63FBE13-A699-ED40-83CD-8E4934AA1AFD}"/>
-    <hyperlink ref="A84" r:id="rId80" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{46C9B508-9149-6B4D-B133-7EA5C8911C80}"/>
-    <hyperlink ref="A85" r:id="rId81" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{BED5C108-0DF5-6F45-904B-056F1FA75509}"/>
-    <hyperlink ref="A86" r:id="rId82" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{CEB3FA5A-F11D-494B-AAF1-B5DAE75E4384}"/>
-    <hyperlink ref="A87" r:id="rId83" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6E426030-FFB0-8345-ACA7-5CD99F72DD37}"/>
-    <hyperlink ref="A88" r:id="rId84" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{292246BE-3177-9A4B-8536-1BEA7FADF7F4}"/>
-    <hyperlink ref="A89" r:id="rId85" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A43045C6-FFAA-0243-85FA-BA84790FD420}"/>
-    <hyperlink ref="A90" r:id="rId86" display="https://www.parkrun.org.uk/sheptonmallet/results/" xr:uid="{8D711C37-EB5D-3F45-AD04-95326C04DA3F}"/>
-    <hyperlink ref="A91" r:id="rId87" display="https://www.parkrun.org.uk/sheptonmallet/results/" xr:uid="{F054E9C3-A29E-FA4F-B80D-7B5023B5DA9A}"/>
-    <hyperlink ref="A92" r:id="rId88" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6829084D-C422-E247-9DF6-3E7821167F39}"/>
-    <hyperlink ref="A93" r:id="rId89" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3F7AAC59-CEF3-214A-BF71-075C44D69479}"/>
-    <hyperlink ref="A94" r:id="rId90" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{895CEF83-5ACD-FB48-8A7E-9B532526B2B1}"/>
-    <hyperlink ref="A95" r:id="rId91" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{200197F8-6E3E-0345-AC83-A63616879D01}"/>
-    <hyperlink ref="A96" r:id="rId92" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A0A51954-76F2-7443-9ABF-EB10E616B31E}"/>
-    <hyperlink ref="A97" r:id="rId93" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3C1B6B9C-6DC8-6849-B993-7194D421BA47}"/>
-    <hyperlink ref="A98" r:id="rId94" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E67BA2ED-9495-4146-8A19-E86863FCEDA9}"/>
-    <hyperlink ref="A99" r:id="rId95" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2A327886-B64E-4546-814D-F558F4B46AEE}"/>
-    <hyperlink ref="A100" r:id="rId96" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E7542DF0-4503-D04B-B108-D83127CFA066}"/>
-    <hyperlink ref="A101" r:id="rId97" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{623015C3-192A-8442-ADE6-9DC87310CB32}"/>
-    <hyperlink ref="A102" r:id="rId98" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{4D2EC9E1-454B-5B4B-A782-C9BE30DA6CF5}"/>
-    <hyperlink ref="A103" r:id="rId99" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{EA583307-6D98-4F42-BC6B-1D2ED2F669D8}"/>
-    <hyperlink ref="A104" r:id="rId100" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{15C9DA90-79C9-4D48-95D4-219CA77B2E1C}"/>
-    <hyperlink ref="A105" r:id="rId101" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{80023DB4-B2B3-B94E-AC16-477C97B312E0}"/>
-    <hyperlink ref="A106" r:id="rId102" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{4F3562B9-0E55-E24E-9BBE-6E08063E2B33}"/>
-    <hyperlink ref="A107" r:id="rId103" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{182D0C11-F9C3-3647-B13F-5FE40608F78B}"/>
-    <hyperlink ref="A108" r:id="rId104" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{57CEFBE2-51A3-4B43-B79E-957C5D32F249}"/>
-    <hyperlink ref="A109" r:id="rId105" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2B0D8668-4F6C-7A43-90EA-0C3B84A5BC8B}"/>
-    <hyperlink ref="A110" r:id="rId106" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{62FDAEB2-59A8-344F-98B3-2E05AE410843}"/>
-    <hyperlink ref="A111" r:id="rId107" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3A4120C1-81DC-2A42-A4BF-FC3E6941E71A}"/>
-    <hyperlink ref="A112" r:id="rId108" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{DE62FFA6-D0CE-9242-AF12-3177536840F3}"/>
-    <hyperlink ref="A113" r:id="rId109" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{047432BE-439F-DC4A-BCE4-2FD5CB6867AC}"/>
-    <hyperlink ref="A114" r:id="rId110" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{146E91EF-9A72-664C-9BCE-BFB4D38F4AA7}"/>
-    <hyperlink ref="A115" r:id="rId111" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{63359FAB-8BA7-D042-AA29-3DF1DF0FB127}"/>
-    <hyperlink ref="A116" r:id="rId112" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{233CE261-263F-3848-A413-0DDAECD785C2}"/>
-    <hyperlink ref="A117" r:id="rId113" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{FE809C0B-C602-5449-8063-33AA34E44813}"/>
-    <hyperlink ref="A118" r:id="rId114" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6666AFCE-0B68-644E-9FFB-2F8818FE9255}"/>
-    <hyperlink ref="A119" r:id="rId115" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{165C9D11-8988-1243-9561-A48B7AE12CA3}"/>
-    <hyperlink ref="A120" r:id="rId116" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{8A21C244-22E5-FD44-991B-B32D7BC525E1}"/>
-    <hyperlink ref="B120" r:id="rId117" display="https://www.parkrun.org.uk/colneylane/results/129/" xr:uid="{BDF93700-E4F5-A14E-9634-356F2857F54B}"/>
-    <hyperlink ref="B119" r:id="rId118" display="https://www.parkrun.org.uk/colneylane/results/130/" xr:uid="{BE1F009A-D283-3F42-B790-70E10821EB19}"/>
-    <hyperlink ref="B118" r:id="rId119" display="https://www.parkrun.org.uk/colneylane/results/145/" xr:uid="{12FC6D48-BB82-0C44-AE67-2955D7F764D4}"/>
-    <hyperlink ref="B117" r:id="rId120" display="https://www.parkrun.org.uk/colneylane/results/146/" xr:uid="{3499EA5B-9DF7-BD4E-98E4-4513B69D2703}"/>
-    <hyperlink ref="B116" r:id="rId121" display="https://www.parkrun.org.uk/colneylane/results/147/" xr:uid="{5C644CBF-9F06-5046-8999-1CBD7034774C}"/>
-    <hyperlink ref="B115" r:id="rId122" display="https://www.parkrun.org.uk/colneylane/results/162/" xr:uid="{94A91BE8-1C74-6D46-B160-52C4BD2E4573}"/>
-    <hyperlink ref="B114" r:id="rId123" display="https://www.parkrun.org.uk/colneylane/results/163/" xr:uid="{5C411B5A-07F3-DA4B-97A0-F72A00B82935}"/>
-    <hyperlink ref="B113" r:id="rId124" display="https://www.parkrun.org.uk/colneylane/results/164/" xr:uid="{B8CEB8B9-E0C6-784E-A1CF-CA84DAF3C50A}"/>
-    <hyperlink ref="B112" r:id="rId125" display="https://www.parkrun.org.uk/colneylane/results/165/" xr:uid="{48B1DE9D-154B-BB4E-B429-D83148F15479}"/>
-    <hyperlink ref="B111" r:id="rId126" display="https://www.parkrun.org.uk/colneylane/results/166/" xr:uid="{DE3D4110-6A44-7246-9900-94E00F1D7889}"/>
-    <hyperlink ref="B110" r:id="rId127" display="https://www.parkrun.org.uk/colneylane/results/172/" xr:uid="{F7B7B294-2667-B24B-AE44-1F0025E79511}"/>
-    <hyperlink ref="B109" r:id="rId128" display="https://www.parkrun.org.uk/colneylane/results/173/" xr:uid="{C8B7124C-ADC0-F249-8769-D8A5A1899C71}"/>
-    <hyperlink ref="B108" r:id="rId129" display="https://www.parkrun.org.uk/colneylane/results/175/" xr:uid="{F27539F9-6B86-F240-96F0-F4E42E518EB8}"/>
-    <hyperlink ref="B107" r:id="rId130" display="https://www.parkrun.org.uk/colneylane/results/176/" xr:uid="{4DE372E5-87B3-1F42-B664-935F5E392799}"/>
-    <hyperlink ref="B106" r:id="rId131" display="https://www.parkrun.org.uk/colneylane/results/177/" xr:uid="{C11B28CD-8526-6041-A9A0-9683F254224F}"/>
-    <hyperlink ref="B105" r:id="rId132" display="https://www.parkrun.org.uk/colneylane/results/178/" xr:uid="{8271D97C-DE25-9F40-9C54-379E0A782E8D}"/>
-    <hyperlink ref="B104" r:id="rId133" display="https://www.parkrun.org.uk/colneylane/results/179/" xr:uid="{4F103D08-DB0B-E745-98F3-C4D71831E642}"/>
-    <hyperlink ref="B103" r:id="rId134" display="https://www.parkrun.org.uk/colneylane/results/180/" xr:uid="{7C6311AA-709A-CA44-BDFB-98FDD33275F7}"/>
-    <hyperlink ref="B102" r:id="rId135" display="https://www.parkrun.org.uk/colneylane/results/181/" xr:uid="{22EBA9FD-1FFF-B640-8661-7A12A5365D41}"/>
-    <hyperlink ref="B101" r:id="rId136" display="https://www.parkrun.org.uk/colneylane/results/182/" xr:uid="{B316186E-A463-304D-8453-F77E8F59524C}"/>
-    <hyperlink ref="B100" r:id="rId137" display="https://www.parkrun.org.uk/colneylane/results/183/" xr:uid="{3EE8F5DE-903F-104E-BFFA-B00573F01381}"/>
-    <hyperlink ref="B99" r:id="rId138" display="https://www.parkrun.org.uk/colneylane/results/184/" xr:uid="{8AB7DD69-0CEF-8142-9C5B-DA9134113CD9}"/>
-    <hyperlink ref="B98" r:id="rId139" display="https://www.parkrun.org.uk/colneylane/results/185/" xr:uid="{CB1D290E-3DE3-A447-A681-E8D568E0FCF4}"/>
-    <hyperlink ref="B97" r:id="rId140" display="https://www.parkrun.org.uk/colneylane/results/186/" xr:uid="{C42AE328-3312-DE4F-B558-526B54C2E356}"/>
-    <hyperlink ref="B96" r:id="rId141" display="https://www.parkrun.org.uk/colneylane/results/187/" xr:uid="{7A725257-A895-D240-B5D1-267602E482AB}"/>
-    <hyperlink ref="B95" r:id="rId142" display="https://www.parkrun.org.uk/colneylane/results/188/" xr:uid="{65DFC959-9C65-7F47-9878-5C5991EC0670}"/>
-    <hyperlink ref="B94" r:id="rId143" display="https://www.parkrun.org.uk/colneylane/results/189/" xr:uid="{658F23E7-5ECD-6041-8AD4-2229508471F9}"/>
-    <hyperlink ref="B93" r:id="rId144" display="https://www.parkrun.org.uk/colneylane/results/190/" xr:uid="{140F819E-6323-3A4E-9568-74DC0102475C}"/>
-    <hyperlink ref="B92" r:id="rId145" display="https://www.parkrun.org.uk/colneylane/results/191/" xr:uid="{12283E4D-6D56-8A49-8D16-347C4D2EDA20}"/>
-    <hyperlink ref="B91" r:id="rId146" display="https://www.parkrun.org.uk/sheptonmallet/results/214/" xr:uid="{F158E6DD-5569-F94F-A29F-6517FD0F3F21}"/>
-    <hyperlink ref="B90" r:id="rId147" display="https://www.parkrun.org.uk/sheptonmallet/results/215/" xr:uid="{1F42BD0C-651A-974C-BFDE-9CB5ED6139D2}"/>
-    <hyperlink ref="B89" r:id="rId148" display="https://www.parkrun.org.uk/colneylane/results/194/" xr:uid="{1AC208E9-B8DB-4D4B-8116-003E7B957AC3}"/>
-    <hyperlink ref="B88" r:id="rId149" display="https://www.parkrun.org.uk/colneylane/results/195/" xr:uid="{F30F367D-B91E-C247-BD5C-80CD62EDB67F}"/>
-    <hyperlink ref="B87" r:id="rId150" display="https://www.parkrun.org.uk/colneylane/results/196/" xr:uid="{1570A655-C8A2-F44F-9957-F907ADD2905C}"/>
-    <hyperlink ref="B86" r:id="rId151" display="https://www.parkrun.org.uk/colneylane/results/197/" xr:uid="{D01824CF-F816-7747-AF06-61788D27D574}"/>
-    <hyperlink ref="B85" r:id="rId152" display="https://www.parkrun.org.uk/colneylane/results/198/" xr:uid="{337334DA-C6E4-8040-97A5-576769C5EC36}"/>
-    <hyperlink ref="B84" r:id="rId153" display="https://www.parkrun.org.uk/colneylane/results/199/" xr:uid="{30DEB108-D1A4-0B41-93BB-7ABCEB9EB266}"/>
-    <hyperlink ref="B83" r:id="rId154" display="https://www.parkrun.org.uk/colneylane/results/200/" xr:uid="{49CC5569-CEF6-904D-8005-FFA90F4C687D}"/>
-    <hyperlink ref="B82" r:id="rId155" display="https://www.parkrun.org.uk/colneylane/results/201/" xr:uid="{5C2479C9-FD4F-B54A-A10D-2C42E4B24488}"/>
-    <hyperlink ref="B81" r:id="rId156" display="https://www.parkrun.org.uk/colneylane/results/202/" xr:uid="{8E47032A-E217-494F-82EA-35E6FCE4B3DA}"/>
-    <hyperlink ref="B80" r:id="rId157" display="https://www.parkrun.org.uk/colneylane/results/203/" xr:uid="{B99B400D-9C64-A442-897F-5AF6E0ECCDCA}"/>
-    <hyperlink ref="B79" r:id="rId158" display="https://www.parkrun.org.uk/colneylane/results/204/" xr:uid="{1FCBB434-91CE-BD4D-B6C5-9AA39128FF86}"/>
-    <hyperlink ref="B78" r:id="rId159" display="https://www.parkrun.org.uk/colneylane/results/205/" xr:uid="{5ACD4D33-E7F4-D744-B9AF-06F3D5E4D526}"/>
-    <hyperlink ref="B77" r:id="rId160" display="https://www.parkrun.org.uk/colneylane/results/206/" xr:uid="{3285115D-CB9D-CC47-87D6-AF03D1880463}"/>
-    <hyperlink ref="B76" r:id="rId161" display="https://www.parkrun.org.uk/colneylane/results/207/" xr:uid="{FDACD0A6-B4B9-3846-8BD6-72CF55EFE920}"/>
-    <hyperlink ref="B75" r:id="rId162" display="https://www.parkrun.org.uk/colneylane/results/208/" xr:uid="{703BB631-758C-6F44-AA64-E556FBCE4F78}"/>
-    <hyperlink ref="B74" r:id="rId163" display="https://www.parkrun.org.uk/colneylane/results/209/" xr:uid="{135AFE44-4000-2D49-963A-622467E6F716}"/>
-    <hyperlink ref="B73" r:id="rId164" display="https://www.parkrun.org.uk/colneylane/results/210/" xr:uid="{68B5C2BF-DB42-9A47-91A4-6189F7762197}"/>
-    <hyperlink ref="B72" r:id="rId165" display="https://www.parkrun.org.uk/colneylane/results/211/" xr:uid="{41A40916-EE52-3F4D-B2A2-F980D70BFEE5}"/>
-    <hyperlink ref="B71" r:id="rId166" display="https://www.parkrun.org.uk/colneylane/results/212/" xr:uid="{03CB32D5-08B2-DC48-A0B9-282534A33E7B}"/>
-    <hyperlink ref="B70" r:id="rId167" display="https://www.parkrun.org.uk/colneylane/results/213/" xr:uid="{ADB5EB1F-CF7D-524B-8AE3-D93FB15B0319}"/>
-    <hyperlink ref="B69" r:id="rId168" display="https://www.parkrun.org.uk/colneylane/results/214/" xr:uid="{9ECE2B28-CF30-9347-B69C-D18B86E08B14}"/>
-    <hyperlink ref="B68" r:id="rId169" display="https://www.parkrun.org.uk/colneylane/results/215/" xr:uid="{C8648389-301B-3847-84A6-88AEB2160221}"/>
-    <hyperlink ref="B67" r:id="rId170" display="https://www.parkrun.org.uk/colneylane/results/216/" xr:uid="{5C554B4B-FD69-AB42-862E-793A2868CCB6}"/>
-    <hyperlink ref="B66" r:id="rId171" display="https://www.parkrun.org.uk/brundall/results/327/" xr:uid="{F2B07DD7-2135-0046-8C1F-F615D4316EF5}"/>
-    <hyperlink ref="B65" r:id="rId172" display="https://www.parkrun.org.uk/colneylane/results/218/" xr:uid="{BC221D90-638D-074D-88E0-A4DFA13E581A}"/>
-    <hyperlink ref="B64" r:id="rId173" display="https://www.parkrun.org.uk/colneylane/results/219/" xr:uid="{CE3427B2-F8AC-CF40-A0E5-4ED8DED7499A}"/>
-    <hyperlink ref="B63" r:id="rId174" display="https://www.parkrun.org.uk/street/results/196/" xr:uid="{A2F90503-5CC1-D648-B412-3D0E5DD025ED}"/>
-    <hyperlink ref="B62" r:id="rId175" display="https://www.parkrun.org.uk/street/results/197/" xr:uid="{9AA629EB-BB94-F644-AA7C-49B78952C9D1}"/>
-    <hyperlink ref="B61" r:id="rId176" display="https://www.parkrun.org.uk/street/results/198/" xr:uid="{A53604FA-93FC-5B44-A2C0-44A1289CD446}"/>
-    <hyperlink ref="B60" r:id="rId177" display="https://www.parkrun.org.uk/norwich/results/607/" xr:uid="{7F30BF94-CE65-D84E-8036-DC7F70E9B957}"/>
-    <hyperlink ref="B59" r:id="rId178" display="https://www.parkrun.org.uk/norwich/results/608/" xr:uid="{01FF343D-AA7B-1247-A875-AACE6444537D}"/>
-    <hyperlink ref="B58" r:id="rId179" display="https://www.parkrun.org.uk/lingwood/results/162/" xr:uid="{81BE335C-A4E9-8F48-9502-960057B3D036}"/>
-    <hyperlink ref="B57" r:id="rId180" display="https://www.parkrun.org.uk/ifieldmillpond/results/130/" xr:uid="{9075B30F-C7DF-4448-A1F1-9E15955B5D5E}"/>
-    <hyperlink ref="B56" r:id="rId181" display="https://www.parkrun.org.uk/thornhamwalks/results/13/" xr:uid="{0A14079D-E818-4C48-AE8C-29E09AE227E2}"/>
-    <hyperlink ref="B55" r:id="rId182" display="https://www.parkrun.org.uk/sloughbottom/results/155/" xr:uid="{05B39168-85DD-FD4B-B58B-137B92289B35}"/>
-    <hyperlink ref="B54" r:id="rId183" display="https://www.parkrun.org.uk/northwalsham/results/79/" xr:uid="{77187675-FE46-8749-B3D1-3FD30605CB78}"/>
-    <hyperlink ref="B53" r:id="rId184" display="https://www.parkrun.org.uk/norwich/results/614/" xr:uid="{F67E4152-65BE-5F42-B04A-778D0E6632D0}"/>
-    <hyperlink ref="B52" r:id="rId185" display="https://www.parkrun.org.uk/lochneaton/results/162/" xr:uid="{66021457-0407-7240-B3CB-1257FD53B00F}"/>
-    <hyperlink ref="B51" r:id="rId186" display="https://www.parkrun.org.uk/colneylane/results/233/" xr:uid="{40CE9E4D-B17C-2841-B71B-7301A5CEF3E9}"/>
-    <hyperlink ref="B50" r:id="rId187" display="https://www.parkrun.org.uk/blickling/results/426/" xr:uid="{E7C04565-8F17-4146-B69B-427E23B8C953}"/>
-    <hyperlink ref="B49" r:id="rId188" display="https://www.parkrun.org.uk/norwich/results/618/" xr:uid="{62B82866-3104-3F41-BA6B-DDFE01A73397}"/>
-    <hyperlink ref="B48" r:id="rId189" display="https://www.parkrun.org.uk/norwich/results/619/" xr:uid="{2C43BD23-53CF-3C44-A168-10E4298A41ED}"/>
-    <hyperlink ref="B47" r:id="rId190" display="https://www.parkrun.org.uk/flegghigh/results/91/" xr:uid="{9F2D5023-3B20-5846-AEB6-2D15A77A4D4B}"/>
-    <hyperlink ref="B46" r:id="rId191" display="https://www.parkrun.org.uk/colneylane/results/238/" xr:uid="{5981EF63-5334-7749-9332-5B326EE3D768}"/>
-    <hyperlink ref="B45" r:id="rId192" display="https://www.parkrun.org.uk/colneylane/results/239/" xr:uid="{F037BF1D-5308-0743-A5A3-ED1943FA0D85}"/>
-    <hyperlink ref="B44" r:id="rId193" display="https://www.parkrun.org.uk/sheringham/results/496/" xr:uid="{4F615B9C-6AB0-7743-B463-CF776025224A}"/>
-    <hyperlink ref="B43" r:id="rId194" display="https://www.parkrun.org.uk/colneylane/results/241/" xr:uid="{6776C435-A98A-E341-A3B8-3568B294B145}"/>
-    <hyperlink ref="B42" r:id="rId195" display="https://www.parkrun.org.uk/thetford/results/505/" xr:uid="{C5DF034E-40D1-3C4A-841D-D2DFA518F6FE}"/>
-    <hyperlink ref="B41" r:id="rId196" display="https://www.parkrun.org.uk/kingslynn/results/575/" xr:uid="{B4B140CA-3E6C-4442-8617-A030F53CA32F}"/>
-    <hyperlink ref="B40" r:id="rId197" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/112/" xr:uid="{2BC101E0-C290-4340-AFC5-35377BD9882B}"/>
-    <hyperlink ref="B39" r:id="rId198" display="https://www.parkrun.org.uk/fivearches/results/15/" xr:uid="{828C921F-AA4C-504E-BDE9-5118EDBF1197}"/>
-    <hyperlink ref="B38" r:id="rId199" display="https://www.parkrun.org.uk/altonwater/results/115/" xr:uid="{7E87F180-D6E4-CA44-846C-D2CFFE4CDC3E}"/>
-    <hyperlink ref="B37" r:id="rId200" display="https://www.parkrun.org.uk/sloughbottom/results/174/" xr:uid="{8331A748-0473-284B-9D3F-147CA024DE3E}"/>
-    <hyperlink ref="B36" r:id="rId201" display="https://www.parkrun.org.uk/catton/results/469/" xr:uid="{2CE95C8B-1FB7-8740-9AE3-AC2972D94120}"/>
-    <hyperlink ref="B35" r:id="rId202" display="https://www.parkrun.org.uk/harlestonmagpies/results/119/" xr:uid="{7CFC187C-1259-BB48-B753-8959174A7930}"/>
-    <hyperlink ref="B34" r:id="rId203" display="https://www.parkrun.org.uk/colneylane/results/249/" xr:uid="{7A8D4EE9-6DAD-C641-BABB-E020B14C8ADB}"/>
-    <hyperlink ref="B33" r:id="rId204" display="https://www.parkrun.org.uk/holkham/results/305/" xr:uid="{2946DD23-45D6-3C4A-8A1F-9A92E2F5EFF3}"/>
-    <hyperlink ref="B32" r:id="rId205" display="https://www.parkrun.org.uk/downhammarketacademy/results/92/" xr:uid="{8E4AA368-9573-2543-B992-B3899538CF99}"/>
-    <hyperlink ref="B31" r:id="rId206" display="https://www.parkrun.org.uk/sloughbottom/results/180/" xr:uid="{311FD894-FC57-F74F-A3C2-C83E6980BD86}"/>
-    <hyperlink ref="B30" r:id="rId207" display="https://www.parkrun.org.uk/brandoncountrypark/results/509/" xr:uid="{BD73B82C-6060-EC46-AF93-C0FEC7BBCBBF}"/>
-    <hyperlink ref="B29" r:id="rId208" display="https://www.parkrun.org.uk/sandringham/results/122/" xr:uid="{12A5795E-4AF7-664B-BEE8-7C9B629721F8}"/>
-    <hyperlink ref="B28" r:id="rId209" display="https://www.parkrun.org.uk/sloughbottom/results/183/" xr:uid="{A5CE83E3-6F97-6849-BB4A-CEFAA53CC597}"/>
-    <hyperlink ref="B27" r:id="rId210" display="https://www.parkrun.org.uk/gorleston/results/706/" xr:uid="{64A72A9B-DC52-204C-AF37-BAFA110BCE6A}"/>
-    <hyperlink ref="B26" r:id="rId211" display="https://www.parkrun.org.uk/sloughbottom/results/185/" xr:uid="{2139748D-B7E9-C841-BB62-6BAED97E9867}"/>
-    <hyperlink ref="B25" r:id="rId212" display="https://www.parkrun.org.uk/gorleston/results/708/" xr:uid="{0703EB07-1E70-4048-ACCF-326FA879ABD5}"/>
-    <hyperlink ref="B24" r:id="rId213" display="https://www.parkrun.org.uk/lowestoft/results/371/" xr:uid="{F8EE4D03-36D9-EF42-B22E-0B557B749314}"/>
-    <hyperlink ref="B23" r:id="rId214" display="https://www.parkrun.org.uk/swaffham/results/239/" xr:uid="{C6D9F588-E9A1-BA4C-9ACE-1EA8CD86F18A}"/>
-    <hyperlink ref="B22" r:id="rId215" display="https://www.parkrun.org.uk/sloughbottom/results/189/" xr:uid="{C83CAE3D-F6EA-A244-9339-34EE0C400C6B}"/>
-    <hyperlink ref="B21" r:id="rId216" display="https://www.parkrun.org.uk/colneylane/results/262/" xr:uid="{CADECC84-9A11-BC40-BBE9-C5932FAB9D67}"/>
-    <hyperlink ref="B20" r:id="rId217" display="https://www.parkrun.org.uk/colneylane/results/263/" xr:uid="{79D3D039-2559-A04E-8636-DECAF17F81BB}"/>
-    <hyperlink ref="B19" r:id="rId218" display="https://www.parkrun.org.uk/sloughbottom/results/192/" xr:uid="{0A93FD3D-30FC-9843-8803-4F54E7F8A3A1}"/>
-    <hyperlink ref="B18" r:id="rId219" display="https://www.parkrun.org.uk/colneylane/results/265/" xr:uid="{A73A411A-B701-2D47-92DE-A8663C135A10}"/>
-    <hyperlink ref="B17" r:id="rId220" display="https://www.parkrun.org.uk/colneylane/results/266/" xr:uid="{8816943F-8C95-1D41-9A07-38EFAEA75902}"/>
-    <hyperlink ref="B16" r:id="rId221" display="https://www.parkrun.org.uk/colneylane/results/267/" xr:uid="{07710C45-F599-1E4D-93E6-F90C7403BBFA}"/>
-    <hyperlink ref="B15" r:id="rId222" display="https://www.parkrun.org.uk/sloughbottom/results/196/" xr:uid="{53E33B80-772A-994D-B8CC-81F4B5E1216C}"/>
-    <hyperlink ref="B14" r:id="rId223" display="https://www.parkrun.org.uk/greatyarmouthnorthbeach/results/152/" xr:uid="{2730402E-D4EF-3B42-8108-749F9C50DBB7}"/>
-    <hyperlink ref="B13" r:id="rId224" display="https://www.parkrun.org.uk/colneylane/results/270/" xr:uid="{E9F2661D-A713-184F-B7D4-2C2E0C4921C8}"/>
-    <hyperlink ref="B12" r:id="rId225" display="https://www.parkrun.org.uk/catton/results/493/" xr:uid="{D6A6D1BB-92BF-C042-B713-DFB2774AA23B}"/>
-    <hyperlink ref="B11" r:id="rId226" display="https://www.parkrun.org.uk/sloughbottom/results/200/" xr:uid="{8338BA8E-B390-DD47-86A2-BC0AC0DE01D4}"/>
-    <hyperlink ref="B10" r:id="rId227" display="https://www.parkrun.org.uk/colneylane/results/273/" xr:uid="{C30BC857-AC17-4F41-BC60-EAA6D83AC68C}"/>
-    <hyperlink ref="B9" r:id="rId228" display="https://www.parkrun.org.uk/colneylane/results/274/" xr:uid="{ADCF8407-F39F-644A-A2D5-5C37714E0B34}"/>
-    <hyperlink ref="B8" r:id="rId229" display="https://www.parkrun.org.uk/sloughbottom/results/203/" xr:uid="{904D2D68-EC1F-ED4A-86A2-98004ABCD0E5}"/>
-    <hyperlink ref="B7" r:id="rId230" display="https://www.parkrun.org.uk/sloughbottom/results/204/" xr:uid="{2758B14F-ECAD-A149-B9CA-DCDDBF51F853}"/>
-    <hyperlink ref="B6" r:id="rId231" display="https://www.parkrun.org.uk/lancingbeachgreen/results/214/" xr:uid="{79550B87-89E2-7041-A9E1-B0215D44BCEB}"/>
-    <hyperlink ref="B5" r:id="rId232" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/142/" xr:uid="{8099819A-DCE9-574A-BE0F-42661BEF8E16}"/>
+    <hyperlink ref="A21" r:id="rId1" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/" xr:uid="{252F5143-8A22-9B42-AF19-A38C76AD6802}"/>
+    <hyperlink ref="A22" r:id="rId2" display="https://www.parkrun.org.uk/lancingbeachgreen/results/" xr:uid="{150F9A52-4040-DA4A-85D2-D42805046243}"/>
+    <hyperlink ref="A23" r:id="rId3" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{BA78F95F-3373-604E-9550-F9E9EF53853F}"/>
+    <hyperlink ref="A24" r:id="rId4" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{40DFFB7F-349A-3149-B170-0BBC7FA11376}"/>
+    <hyperlink ref="A25" r:id="rId5" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{AA4429C8-98C4-3547-BFC6-C557606F2095}"/>
+    <hyperlink ref="A26" r:id="rId6" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B59B6240-6A79-F840-B20F-17478D063E0C}"/>
+    <hyperlink ref="A27" r:id="rId7" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{A6747A4E-8473-ED4B-A863-3C1462B63A87}"/>
+    <hyperlink ref="A28" r:id="rId8" display="https://www.parkrun.org.uk/catton/results/" xr:uid="{E3235270-25A9-9742-AC78-C6FB78EB746A}"/>
+    <hyperlink ref="A29" r:id="rId9" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3308C1A0-1C47-0C45-AD10-E078B08E84FC}"/>
+    <hyperlink ref="A30" r:id="rId10" display="https://www.parkrun.org.uk/greatyarmouthnorthbeach/results/" xr:uid="{E2A8AE47-AEA1-E44E-A199-19E11D7701DB}"/>
+    <hyperlink ref="A31" r:id="rId11" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{D9F72049-A833-0843-8159-D44B0C17A0F2}"/>
+    <hyperlink ref="A32" r:id="rId12" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6CA9A3C6-9033-2D44-B763-080A52A3718E}"/>
+    <hyperlink ref="A33" r:id="rId13" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B948A7B6-701C-874F-AD10-52310D121ECF}"/>
+    <hyperlink ref="A34" r:id="rId14" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{5F6095C9-2D81-2041-AF22-39BB4B6E1FA1}"/>
+    <hyperlink ref="A35" r:id="rId15" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{20872887-70C5-8049-B79C-D77851A224BE}"/>
+    <hyperlink ref="A36" r:id="rId16" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{61B7BAE3-6120-C244-933B-74AFEB167CB2}"/>
+    <hyperlink ref="A37" r:id="rId17" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{77B35723-636C-414F-8CEA-21D73264A764}"/>
+    <hyperlink ref="A38" r:id="rId18" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{504E6E96-07D3-C940-972F-02BCFE77CD66}"/>
+    <hyperlink ref="A39" r:id="rId19" display="https://www.parkrun.org.uk/swaffham/results/" xr:uid="{F7E130F9-71A3-034A-BCD8-9C5433C3D2F2}"/>
+    <hyperlink ref="A40" r:id="rId20" display="https://www.parkrun.org.uk/lowestoft/results/" xr:uid="{CBBA3CCB-DE8F-FA4C-876C-F56FD93D48FE}"/>
+    <hyperlink ref="A41" r:id="rId21" display="https://www.parkrun.org.uk/gorleston/results/" xr:uid="{D19FD83E-B7F7-634D-B167-462C567C2D4C}"/>
+    <hyperlink ref="A42" r:id="rId22" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{8519BDAB-3B2D-E944-8BE3-918E6C2F0EC5}"/>
+    <hyperlink ref="A43" r:id="rId23" display="https://www.parkrun.org.uk/gorleston/results/" xr:uid="{98AAA3A6-E767-3645-8D46-91EDBE0F0041}"/>
+    <hyperlink ref="A44" r:id="rId24" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{FDC42F18-28C5-9544-9F4E-861278ECB8EC}"/>
+    <hyperlink ref="A45" r:id="rId25" display="https://www.parkrun.org.uk/sandringham/results/" xr:uid="{925F3C71-F640-9543-AA11-78FDAE8F1988}"/>
+    <hyperlink ref="A46" r:id="rId26" display="https://www.parkrun.org.uk/brandoncountrypark/results/" xr:uid="{E77E37E4-D552-014F-95E9-94839E4DC9E7}"/>
+    <hyperlink ref="A47" r:id="rId27" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{E67019B4-05BA-9C48-9D0B-4D7996ACADDE}"/>
+    <hyperlink ref="A48" r:id="rId28" display="https://www.parkrun.org.uk/downhammarketacademy/results/" xr:uid="{4B14F13C-9004-8E49-9644-330FC85E3187}"/>
+    <hyperlink ref="A49" r:id="rId29" display="https://www.parkrun.org.uk/holkham/results/" xr:uid="{D1D42CE4-1B9D-A347-A668-27648D573172}"/>
+    <hyperlink ref="A50" r:id="rId30" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{F7EFF658-EC1C-7B4E-92FD-5F07789417A2}"/>
+    <hyperlink ref="A51" r:id="rId31" display="https://www.parkrun.org.uk/harlestonmagpies/results/" xr:uid="{5A43BF3F-61E2-084B-A1EB-AA9F3FE90FA2}"/>
+    <hyperlink ref="A52" r:id="rId32" display="https://www.parkrun.org.uk/catton/results/" xr:uid="{DE7DFFB6-7932-3D44-B06E-9FF86D65E128}"/>
+    <hyperlink ref="A53" r:id="rId33" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{D36393C6-CDF1-B541-919C-20BB8B44A055}"/>
+    <hyperlink ref="A54" r:id="rId34" display="https://www.parkrun.org.uk/altonwater/results/" xr:uid="{B49D816D-65CD-6345-AF36-8F5D2D6F2DD2}"/>
+    <hyperlink ref="A55" r:id="rId35" display="https://www.parkrun.org.uk/fivearches/results/" xr:uid="{DF90DA80-328B-1F4E-AD0D-451881682315}"/>
+    <hyperlink ref="A56" r:id="rId36" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/" xr:uid="{D67D01BA-A614-BC47-A357-5DEE330A639A}"/>
+    <hyperlink ref="A57" r:id="rId37" display="https://www.parkrun.org.uk/kingslynn/results/" xr:uid="{9B3D9FAB-2F2B-F04D-B98B-86A237E8BEFE}"/>
+    <hyperlink ref="A58" r:id="rId38" display="https://www.parkrun.org.uk/thetford/results/" xr:uid="{0173A15B-333E-5A4A-89FF-CFAF8CB0A408}"/>
+    <hyperlink ref="A59" r:id="rId39" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{845864C9-A5AA-FB4E-B257-7EAD70D2A84F}"/>
+    <hyperlink ref="A60" r:id="rId40" display="https://www.parkrun.org.uk/sheringham/results/" xr:uid="{365454C0-82CB-3F4F-8C1E-9C3A3998F3C0}"/>
+    <hyperlink ref="A61" r:id="rId41" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2E6F02C3-E788-8F44-99AB-6C806F37B49C}"/>
+    <hyperlink ref="A62" r:id="rId42" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{038CCF2F-9AE8-254D-8881-FDF710086E84}"/>
+    <hyperlink ref="A63" r:id="rId43" display="https://www.parkrun.org.uk/flegghigh/results/" xr:uid="{56BC7901-47C2-3145-8BBB-FFF3DE713576}"/>
+    <hyperlink ref="A64" r:id="rId44" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{4FC66B5F-2CE0-2247-A578-3992703E9896}"/>
+    <hyperlink ref="A65" r:id="rId45" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{5E398874-BF44-4344-9D7C-3C99BAFDB2A8}"/>
+    <hyperlink ref="A66" r:id="rId46" display="https://www.parkrun.org.uk/blickling/results/" xr:uid="{801E4171-29D4-EF4B-8E64-4A363FEC37C1}"/>
+    <hyperlink ref="A67" r:id="rId47" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{1467205D-F890-3C4F-833C-5F20EAA517A1}"/>
+    <hyperlink ref="A68" r:id="rId48" display="https://www.parkrun.org.uk/lochneaton/results/" xr:uid="{E33089F3-68BD-1E44-A176-6BCC42EBD3D5}"/>
+    <hyperlink ref="A69" r:id="rId49" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{380AB618-03F9-A94F-9D0A-E87743178E6B}"/>
+    <hyperlink ref="A70" r:id="rId50" display="https://www.parkrun.org.uk/northwalsham/results/" xr:uid="{BD0A4B75-0054-F844-A891-406B46E42F7B}"/>
+    <hyperlink ref="A71" r:id="rId51" display="https://www.parkrun.org.uk/sloughbottom/results/" xr:uid="{16ECAEF5-D501-214E-BB0B-AD9526B41263}"/>
+    <hyperlink ref="A72" r:id="rId52" display="https://www.parkrun.org.uk/thornhamwalks/results/" xr:uid="{30AF7899-6690-5D4C-89D6-AD2ADB364F33}"/>
+    <hyperlink ref="A73" r:id="rId53" display="https://www.parkrun.org.uk/ifieldmillpond/results/" xr:uid="{0F571825-498D-AC4A-A040-E5834134979F}"/>
+    <hyperlink ref="A74" r:id="rId54" display="https://www.parkrun.org.uk/lingwood/results/" xr:uid="{764330BE-DC68-2E4E-8734-7D93450DFB66}"/>
+    <hyperlink ref="A75" r:id="rId55" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{CA96D4E5-6490-B848-A17A-FF069DC8604A}"/>
+    <hyperlink ref="A76" r:id="rId56" display="https://www.parkrun.org.uk/norwich/results/" xr:uid="{D0C1E86A-C330-DB40-BAA0-77264FCE0C23}"/>
+    <hyperlink ref="A77" r:id="rId57" display="https://www.parkrun.org.uk/street/results/" xr:uid="{F3B8A3FF-6369-AF41-BE95-9530C386002F}"/>
+    <hyperlink ref="A78" r:id="rId58" display="https://www.parkrun.org.uk/street/results/" xr:uid="{8CCE05DF-2116-3A42-A504-4DFAFC3EB05D}"/>
+    <hyperlink ref="A79" r:id="rId59" display="https://www.parkrun.org.uk/street/results/" xr:uid="{4E54B80E-A3E6-104B-9375-403534648F81}"/>
+    <hyperlink ref="A80" r:id="rId60" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{48C5576D-0058-2E48-9CC2-C287C64176C0}"/>
+    <hyperlink ref="A81" r:id="rId61" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{65B5A2BE-625A-C344-82F9-CC7E7572E2C8}"/>
+    <hyperlink ref="A82" r:id="rId62" display="https://www.parkrun.org.uk/brundall/results/" xr:uid="{F1B54B20-A89D-4746-975A-93D721F6B098}"/>
+    <hyperlink ref="A83" r:id="rId63" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A817D26B-6260-4D43-8B48-C501D9B554DA}"/>
+    <hyperlink ref="A84" r:id="rId64" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{8FEB1C36-5771-254F-A34B-81B6E0B0E92B}"/>
+    <hyperlink ref="A85" r:id="rId65" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{07BE9A8E-E930-314E-88B5-6B403477CC9B}"/>
+    <hyperlink ref="A86" r:id="rId66" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{86F146B6-D354-8049-A03B-C534E7126A50}"/>
+    <hyperlink ref="A87" r:id="rId67" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{1AF8CE9C-E6F3-BC49-A37C-703F79801090}"/>
+    <hyperlink ref="A88" r:id="rId68" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{537CF7E1-771F-F140-90CA-167E905B8DB7}"/>
+    <hyperlink ref="A89" r:id="rId69" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{9DB1979F-9A6F-6846-9E9B-15C948E6086E}"/>
+    <hyperlink ref="A90" r:id="rId70" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{94DCDC74-0483-914F-AE56-14F015F17617}"/>
+    <hyperlink ref="A91" r:id="rId71" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{98BFC344-5F98-2142-BF8B-BB64DC5DC176}"/>
+    <hyperlink ref="A92" r:id="rId72" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{152159AF-1135-ED49-A618-642813444F0B}"/>
+    <hyperlink ref="A93" r:id="rId73" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{782991EE-775E-1546-AC50-21A63A97DED3}"/>
+    <hyperlink ref="A94" r:id="rId74" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3AA8F00C-5402-EE44-812C-82FD37A2D123}"/>
+    <hyperlink ref="A95" r:id="rId75" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A620B43D-EFB5-7248-BED3-BB4F86A9B6CE}"/>
+    <hyperlink ref="A96" r:id="rId76" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{705246F0-97DB-F14C-8CBE-C6F161F61999}"/>
+    <hyperlink ref="A97" r:id="rId77" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{C9B996B1-3496-1B41-8B36-E0C135D5852E}"/>
+    <hyperlink ref="A98" r:id="rId78" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{B3F85754-A195-B04D-AA5B-9CA78330AF14}"/>
+    <hyperlink ref="A99" r:id="rId79" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E63FBE13-A699-ED40-83CD-8E4934AA1AFD}"/>
+    <hyperlink ref="A100" r:id="rId80" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{46C9B508-9149-6B4D-B133-7EA5C8911C80}"/>
+    <hyperlink ref="A101" r:id="rId81" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{BED5C108-0DF5-6F45-904B-056F1FA75509}"/>
+    <hyperlink ref="A102" r:id="rId82" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{CEB3FA5A-F11D-494B-AAF1-B5DAE75E4384}"/>
+    <hyperlink ref="A103" r:id="rId83" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6E426030-FFB0-8345-ACA7-5CD99F72DD37}"/>
+    <hyperlink ref="A104" r:id="rId84" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{292246BE-3177-9A4B-8536-1BEA7FADF7F4}"/>
+    <hyperlink ref="A105" r:id="rId85" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A43045C6-FFAA-0243-85FA-BA84790FD420}"/>
+    <hyperlink ref="A106" r:id="rId86" display="https://www.parkrun.org.uk/sheptonmallet/results/" xr:uid="{8D711C37-EB5D-3F45-AD04-95326C04DA3F}"/>
+    <hyperlink ref="A107" r:id="rId87" display="https://www.parkrun.org.uk/sheptonmallet/results/" xr:uid="{F054E9C3-A29E-FA4F-B80D-7B5023B5DA9A}"/>
+    <hyperlink ref="A108" r:id="rId88" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6829084D-C422-E247-9DF6-3E7821167F39}"/>
+    <hyperlink ref="A109" r:id="rId89" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3F7AAC59-CEF3-214A-BF71-075C44D69479}"/>
+    <hyperlink ref="A110" r:id="rId90" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{895CEF83-5ACD-FB48-8A7E-9B532526B2B1}"/>
+    <hyperlink ref="A111" r:id="rId91" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{200197F8-6E3E-0345-AC83-A63616879D01}"/>
+    <hyperlink ref="A112" r:id="rId92" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{A0A51954-76F2-7443-9ABF-EB10E616B31E}"/>
+    <hyperlink ref="A113" r:id="rId93" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3C1B6B9C-6DC8-6849-B993-7194D421BA47}"/>
+    <hyperlink ref="A114" r:id="rId94" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E67BA2ED-9495-4146-8A19-E86863FCEDA9}"/>
+    <hyperlink ref="A115" r:id="rId95" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2A327886-B64E-4546-814D-F558F4B46AEE}"/>
+    <hyperlink ref="A116" r:id="rId96" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{E7542DF0-4503-D04B-B108-D83127CFA066}"/>
+    <hyperlink ref="A117" r:id="rId97" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{623015C3-192A-8442-ADE6-9DC87310CB32}"/>
+    <hyperlink ref="A118" r:id="rId98" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{4D2EC9E1-454B-5B4B-A782-C9BE30DA6CF5}"/>
+    <hyperlink ref="A119" r:id="rId99" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{EA583307-6D98-4F42-BC6B-1D2ED2F669D8}"/>
+    <hyperlink ref="A120" r:id="rId100" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{15C9DA90-79C9-4D48-95D4-219CA77B2E1C}"/>
+    <hyperlink ref="A121" r:id="rId101" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{80023DB4-B2B3-B94E-AC16-477C97B312E0}"/>
+    <hyperlink ref="A122" r:id="rId102" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{4F3562B9-0E55-E24E-9BBE-6E08063E2B33}"/>
+    <hyperlink ref="A123" r:id="rId103" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{182D0C11-F9C3-3647-B13F-5FE40608F78B}"/>
+    <hyperlink ref="A124" r:id="rId104" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{57CEFBE2-51A3-4B43-B79E-957C5D32F249}"/>
+    <hyperlink ref="A125" r:id="rId105" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{2B0D8668-4F6C-7A43-90EA-0C3B84A5BC8B}"/>
+    <hyperlink ref="A126" r:id="rId106" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{62FDAEB2-59A8-344F-98B3-2E05AE410843}"/>
+    <hyperlink ref="A127" r:id="rId107" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{3A4120C1-81DC-2A42-A4BF-FC3E6941E71A}"/>
+    <hyperlink ref="A128" r:id="rId108" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{DE62FFA6-D0CE-9242-AF12-3177536840F3}"/>
+    <hyperlink ref="A129" r:id="rId109" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{047432BE-439F-DC4A-BCE4-2FD5CB6867AC}"/>
+    <hyperlink ref="A130" r:id="rId110" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{146E91EF-9A72-664C-9BCE-BFB4D38F4AA7}"/>
+    <hyperlink ref="A131" r:id="rId111" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{63359FAB-8BA7-D042-AA29-3DF1DF0FB127}"/>
+    <hyperlink ref="A132" r:id="rId112" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{233CE261-263F-3848-A413-0DDAECD785C2}"/>
+    <hyperlink ref="A133" r:id="rId113" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{FE809C0B-C602-5449-8063-33AA34E44813}"/>
+    <hyperlink ref="A134" r:id="rId114" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{6666AFCE-0B68-644E-9FFB-2F8818FE9255}"/>
+    <hyperlink ref="A135" r:id="rId115" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{165C9D11-8988-1243-9561-A48B7AE12CA3}"/>
+    <hyperlink ref="A136" r:id="rId116" display="https://www.parkrun.org.uk/colneylane/results/" xr:uid="{8A21C244-22E5-FD44-991B-B32D7BC525E1}"/>
+    <hyperlink ref="B136" r:id="rId117" display="https://www.parkrun.org.uk/colneylane/results/129/" xr:uid="{BDF93700-E4F5-A14E-9634-356F2857F54B}"/>
+    <hyperlink ref="B135" r:id="rId118" display="https://www.parkrun.org.uk/colneylane/results/130/" xr:uid="{BE1F009A-D283-3F42-B790-70E10821EB19}"/>
+    <hyperlink ref="B134" r:id="rId119" display="https://www.parkrun.org.uk/colneylane/results/145/" xr:uid="{12FC6D48-BB82-0C44-AE67-2955D7F764D4}"/>
+    <hyperlink ref="B133" r:id="rId120" display="https://www.parkrun.org.uk/colneylane/results/146/" xr:uid="{3499EA5B-9DF7-BD4E-98E4-4513B69D2703}"/>
+    <hyperlink ref="B132" r:id="rId121" display="https://www.parkrun.org.uk/colneylane/results/147/" xr:uid="{5C644CBF-9F06-5046-8999-1CBD7034774C}"/>
+    <hyperlink ref="B131" r:id="rId122" display="https://www.parkrun.org.uk/colneylane/results/162/" xr:uid="{94A91BE8-1C74-6D46-B160-52C4BD2E4573}"/>
+    <hyperlink ref="B130" r:id="rId123" display="https://www.parkrun.org.uk/colneylane/results/163/" xr:uid="{5C411B5A-07F3-DA4B-97A0-F72A00B82935}"/>
+    <hyperlink ref="B129" r:id="rId124" display="https://www.parkrun.org.uk/colneylane/results/164/" xr:uid="{B8CEB8B9-E0C6-784E-A1CF-CA84DAF3C50A}"/>
+    <hyperlink ref="B128" r:id="rId125" display="https://www.parkrun.org.uk/colneylane/results/165/" xr:uid="{48B1DE9D-154B-BB4E-B429-D83148F15479}"/>
+    <hyperlink ref="B127" r:id="rId126" display="https://www.parkrun.org.uk/colneylane/results/166/" xr:uid="{DE3D4110-6A44-7246-9900-94E00F1D7889}"/>
+    <hyperlink ref="B126" r:id="rId127" display="https://www.parkrun.org.uk/colneylane/results/172/" xr:uid="{F7B7B294-2667-B24B-AE44-1F0025E79511}"/>
+    <hyperlink ref="B125" r:id="rId128" display="https://www.parkrun.org.uk/colneylane/results/173/" xr:uid="{C8B7124C-ADC0-F249-8769-D8A5A1899C71}"/>
+    <hyperlink ref="B124" r:id="rId129" display="https://www.parkrun.org.uk/colneylane/results/175/" xr:uid="{F27539F9-6B86-F240-96F0-F4E42E518EB8}"/>
+    <hyperlink ref="B123" r:id="rId130" display="https://www.parkrun.org.uk/colneylane/results/176/" xr:uid="{4DE372E5-87B3-1F42-B664-935F5E392799}"/>
+    <hyperlink ref="B122" r:id="rId131" display="https://www.parkrun.org.uk/colneylane/results/177/" xr:uid="{C11B28CD-8526-6041-A9A0-9683F254224F}"/>
+    <hyperlink ref="B121" r:id="rId132" display="https://www.parkrun.org.uk/colneylane/results/178/" xr:uid="{8271D97C-DE25-9F40-9C54-379E0A782E8D}"/>
+    <hyperlink ref="B120" r:id="rId133" display="https://www.parkrun.org.uk/colneylane/results/179/" xr:uid="{4F103D08-DB0B-E745-98F3-C4D71831E642}"/>
+    <hyperlink ref="B119" r:id="rId134" display="https://www.parkrun.org.uk/colneylane/results/180/" xr:uid="{7C6311AA-709A-CA44-BDFB-98FDD33275F7}"/>
+    <hyperlink ref="B118" r:id="rId135" display="https://www.parkrun.org.uk/colneylane/results/181/" xr:uid="{22EBA9FD-1FFF-B640-8661-7A12A5365D41}"/>
+    <hyperlink ref="B117" r:id="rId136" display="https://www.parkrun.org.uk/colneylane/results/182/" xr:uid="{B316186E-A463-304D-8453-F77E8F59524C}"/>
+    <hyperlink ref="B116" r:id="rId137" display="https://www.parkrun.org.uk/colneylane/results/183/" xr:uid="{3EE8F5DE-903F-104E-BFFA-B00573F01381}"/>
+    <hyperlink ref="B115" r:id="rId138" display="https://www.parkrun.org.uk/colneylane/results/184/" xr:uid="{8AB7DD69-0CEF-8142-9C5B-DA9134113CD9}"/>
+    <hyperlink ref="B114" r:id="rId139" display="https://www.parkrun.org.uk/colneylane/results/185/" xr:uid="{CB1D290E-3DE3-A447-A681-E8D568E0FCF4}"/>
+    <hyperlink ref="B113" r:id="rId140" display="https://www.parkrun.org.uk/colneylane/results/186/" xr:uid="{C42AE328-3312-DE4F-B558-526B54C2E356}"/>
+    <hyperlink ref="B112" r:id="rId141" display="https://www.parkrun.org.uk/colneylane/results/187/" xr:uid="{7A725257-A895-D240-B5D1-267602E482AB}"/>
+    <hyperlink ref="B111" r:id="rId142" display="https://www.parkrun.org.uk/colneylane/results/188/" xr:uid="{65DFC959-9C65-7F47-9878-5C5991EC0670}"/>
+    <hyperlink ref="B110" r:id="rId143" display="https://www.parkrun.org.uk/colneylane/results/189/" xr:uid="{658F23E7-5ECD-6041-8AD4-2229508471F9}"/>
+    <hyperlink ref="B109" r:id="rId144" display="https://www.parkrun.org.uk/colneylane/results/190/" xr:uid="{140F819E-6323-3A4E-9568-74DC0102475C}"/>
+    <hyperlink ref="B108" r:id="rId145" display="https://www.parkrun.org.uk/colneylane/results/191/" xr:uid="{12283E4D-6D56-8A49-8D16-347C4D2EDA20}"/>
+    <hyperlink ref="B107" r:id="rId146" display="https://www.parkrun.org.uk/sheptonmallet/results/214/" xr:uid="{F158E6DD-5569-F94F-A29F-6517FD0F3F21}"/>
+    <hyperlink ref="B106" r:id="rId147" display="https://www.parkrun.org.uk/sheptonmallet/results/215/" xr:uid="{1F42BD0C-651A-974C-BFDE-9CB5ED6139D2}"/>
+    <hyperlink ref="B105" r:id="rId148" display="https://www.parkrun.org.uk/colneylane/results/194/" xr:uid="{1AC208E9-B8DB-4D4B-8116-003E7B957AC3}"/>
+    <hyperlink ref="B104" r:id="rId149" display="https://www.parkrun.org.uk/colneylane/results/195/" xr:uid="{F30F367D-B91E-C247-BD5C-80CD62EDB67F}"/>
+    <hyperlink ref="B103" r:id="rId150" display="https://www.parkrun.org.uk/colneylane/results/196/" xr:uid="{1570A655-C8A2-F44F-9957-F907ADD2905C}"/>
+    <hyperlink ref="B102" r:id="rId151" display="https://www.parkrun.org.uk/colneylane/results/197/" xr:uid="{D01824CF-F816-7747-AF06-61788D27D574}"/>
+    <hyperlink ref="B101" r:id="rId152" display="https://www.parkrun.org.uk/colneylane/results/198/" xr:uid="{337334DA-C6E4-8040-97A5-576769C5EC36}"/>
+    <hyperlink ref="B100" r:id="rId153" display="https://www.parkrun.org.uk/colneylane/results/199/" xr:uid="{30DEB108-D1A4-0B41-93BB-7ABCEB9EB266}"/>
+    <hyperlink ref="B99" r:id="rId154" display="https://www.parkrun.org.uk/colneylane/results/200/" xr:uid="{49CC5569-CEF6-904D-8005-FFA90F4C687D}"/>
+    <hyperlink ref="B98" r:id="rId155" display="https://www.parkrun.org.uk/colneylane/results/201/" xr:uid="{5C2479C9-FD4F-B54A-A10D-2C42E4B24488}"/>
+    <hyperlink ref="B97" r:id="rId156" display="https://www.parkrun.org.uk/colneylane/results/202/" xr:uid="{8E47032A-E217-494F-82EA-35E6FCE4B3DA}"/>
+    <hyperlink ref="B96" r:id="rId157" display="https://www.parkrun.org.uk/colneylane/results/203/" xr:uid="{B99B400D-9C64-A442-897F-5AF6E0ECCDCA}"/>
+    <hyperlink ref="B95" r:id="rId158" display="https://www.parkrun.org.uk/colneylane/results/204/" xr:uid="{1FCBB434-91CE-BD4D-B6C5-9AA39128FF86}"/>
+    <hyperlink ref="B94" r:id="rId159" display="https://www.parkrun.org.uk/colneylane/results/205/" xr:uid="{5ACD4D33-E7F4-D744-B9AF-06F3D5E4D526}"/>
+    <hyperlink ref="B93" r:id="rId160" display="https://www.parkrun.org.uk/colneylane/results/206/" xr:uid="{3285115D-CB9D-CC47-87D6-AF03D1880463}"/>
+    <hyperlink ref="B92" r:id="rId161" display="https://www.parkrun.org.uk/colneylane/results/207/" xr:uid="{FDACD0A6-B4B9-3846-8BD6-72CF55EFE920}"/>
+    <hyperlink ref="B91" r:id="rId162" display="https://www.parkrun.org.uk/colneylane/results/208/" xr:uid="{703BB631-758C-6F44-AA64-E556FBCE4F78}"/>
+    <hyperlink ref="B90" r:id="rId163" display="https://www.parkrun.org.uk/colneylane/results/209/" xr:uid="{135AFE44-4000-2D49-963A-622467E6F716}"/>
+    <hyperlink ref="B89" r:id="rId164" display="https://www.parkrun.org.uk/colneylane/results/210/" xr:uid="{68B5C2BF-DB42-9A47-91A4-6189F7762197}"/>
+    <hyperlink ref="B88" r:id="rId165" display="https://www.parkrun.org.uk/colneylane/results/211/" xr:uid="{41A40916-EE52-3F4D-B2A2-F980D70BFEE5}"/>
+    <hyperlink ref="B87" r:id="rId166" display="https://www.parkrun.org.uk/colneylane/results/212/" xr:uid="{03CB32D5-08B2-DC48-A0B9-282534A33E7B}"/>
+    <hyperlink ref="B86" r:id="rId167" display="https://www.parkrun.org.uk/colneylane/results/213/" xr:uid="{ADB5EB1F-CF7D-524B-8AE3-D93FB15B0319}"/>
+    <hyperlink ref="B85" r:id="rId168" display="https://www.parkrun.org.uk/colneylane/results/214/" xr:uid="{9ECE2B28-CF30-9347-B69C-D18B86E08B14}"/>
+    <hyperlink ref="B84" r:id="rId169" display="https://www.parkrun.org.uk/colneylane/results/215/" xr:uid="{C8648389-301B-3847-84A6-88AEB2160221}"/>
+    <hyperlink ref="B83" r:id="rId170" display="https://www.parkrun.org.uk/colneylane/results/216/" xr:uid="{5C554B4B-FD69-AB42-862E-793A2868CCB6}"/>
+    <hyperlink ref="B82" r:id="rId171" display="https://www.parkrun.org.uk/brundall/results/327/" xr:uid="{F2B07DD7-2135-0046-8C1F-F615D4316EF5}"/>
+    <hyperlink ref="B81" r:id="rId172" display="https://www.parkrun.org.uk/colneylane/results/218/" xr:uid="{BC221D90-638D-074D-88E0-A4DFA13E581A}"/>
+    <hyperlink ref="B80" r:id="rId173" display="https://www.parkrun.org.uk/colneylane/results/219/" xr:uid="{CE3427B2-F8AC-CF40-A0E5-4ED8DED7499A}"/>
+    <hyperlink ref="B79" r:id="rId174" display="https://www.parkrun.org.uk/street/results/196/" xr:uid="{A2F90503-5CC1-D648-B412-3D0E5DD025ED}"/>
+    <hyperlink ref="B78" r:id="rId175" display="https://www.parkrun.org.uk/street/results/197/" xr:uid="{9AA629EB-BB94-F644-AA7C-49B78952C9D1}"/>
+    <hyperlink ref="B77" r:id="rId176" display="https://www.parkrun.org.uk/street/results/198/" xr:uid="{A53604FA-93FC-5B44-A2C0-44A1289CD446}"/>
+    <hyperlink ref="B76" r:id="rId177" display="https://www.parkrun.org.uk/norwich/results/607/" xr:uid="{7F30BF94-CE65-D84E-8036-DC7F70E9B957}"/>
+    <hyperlink ref="B75" r:id="rId178" display="https://www.parkrun.org.uk/norwich/results/608/" xr:uid="{01FF343D-AA7B-1247-A875-AACE6444537D}"/>
+    <hyperlink ref="B74" r:id="rId179" display="https://www.parkrun.org.uk/lingwood/results/162/" xr:uid="{81BE335C-A4E9-8F48-9502-960057B3D036}"/>
+    <hyperlink ref="B73" r:id="rId180" display="https://www.parkrun.org.uk/ifieldmillpond/results/130/" xr:uid="{9075B30F-C7DF-4448-A1F1-9E15955B5D5E}"/>
+    <hyperlink ref="B72" r:id="rId181" display="https://www.parkrun.org.uk/thornhamwalks/results/13/" xr:uid="{0A14079D-E818-4C48-AE8C-29E09AE227E2}"/>
+    <hyperlink ref="B71" r:id="rId182" display="https://www.parkrun.org.uk/sloughbottom/results/155/" xr:uid="{05B39168-85DD-FD4B-B58B-137B92289B35}"/>
+    <hyperlink ref="B70" r:id="rId183" display="https://www.parkrun.org.uk/northwalsham/results/79/" xr:uid="{77187675-FE46-8749-B3D1-3FD30605CB78}"/>
+    <hyperlink ref="B69" r:id="rId184" display="https://www.parkrun.org.uk/norwich/results/614/" xr:uid="{F67E4152-65BE-5F42-B04A-778D0E6632D0}"/>
+    <hyperlink ref="B68" r:id="rId185" display="https://www.parkrun.org.uk/lochneaton/results/162/" xr:uid="{66021457-0407-7240-B3CB-1257FD53B00F}"/>
+    <hyperlink ref="B67" r:id="rId186" display="https://www.parkrun.org.uk/colneylane/results/233/" xr:uid="{40CE9E4D-B17C-2841-B71B-7301A5CEF3E9}"/>
+    <hyperlink ref="B66" r:id="rId187" display="https://www.parkrun.org.uk/blickling/results/426/" xr:uid="{E7C04565-8F17-4146-B69B-427E23B8C953}"/>
+    <hyperlink ref="B65" r:id="rId188" display="https://www.parkrun.org.uk/norwich/results/618/" xr:uid="{62B82866-3104-3F41-BA6B-DDFE01A73397}"/>
+    <hyperlink ref="B64" r:id="rId189" display="https://www.parkrun.org.uk/norwich/results/619/" xr:uid="{2C43BD23-53CF-3C44-A168-10E4298A41ED}"/>
+    <hyperlink ref="B63" r:id="rId190" display="https://www.parkrun.org.uk/flegghigh/results/91/" xr:uid="{9F2D5023-3B20-5846-AEB6-2D15A77A4D4B}"/>
+    <hyperlink ref="B62" r:id="rId191" display="https://www.parkrun.org.uk/colneylane/results/238/" xr:uid="{5981EF63-5334-7749-9332-5B326EE3D768}"/>
+    <hyperlink ref="B61" r:id="rId192" display="https://www.parkrun.org.uk/colneylane/results/239/" xr:uid="{F037BF1D-5308-0743-A5A3-ED1943FA0D85}"/>
+    <hyperlink ref="B60" r:id="rId193" display="https://www.parkrun.org.uk/sheringham/results/496/" xr:uid="{4F615B9C-6AB0-7743-B463-CF776025224A}"/>
+    <hyperlink ref="B59" r:id="rId194" display="https://www.parkrun.org.uk/colneylane/results/241/" xr:uid="{6776C435-A98A-E341-A3B8-3568B294B145}"/>
+    <hyperlink ref="B58" r:id="rId195" display="https://www.parkrun.org.uk/thetford/results/505/" xr:uid="{C5DF034E-40D1-3C4A-841D-D2DFA518F6FE}"/>
+    <hyperlink ref="B57" r:id="rId196" display="https://www.parkrun.org.uk/kingslynn/results/575/" xr:uid="{B4B140CA-3E6C-4442-8617-A030F53CA32F}"/>
+    <hyperlink ref="B56" r:id="rId197" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/112/" xr:uid="{2BC101E0-C290-4340-AFC5-35377BD9882B}"/>
+    <hyperlink ref="B55" r:id="rId198" display="https://www.parkrun.org.uk/fivearches/results/15/" xr:uid="{828C921F-AA4C-504E-BDE9-5118EDBF1197}"/>
+    <hyperlink ref="B54" r:id="rId199" display="https://www.parkrun.org.uk/altonwater/results/115/" xr:uid="{7E87F180-D6E4-CA44-846C-D2CFFE4CDC3E}"/>
+    <hyperlink ref="B53" r:id="rId200" display="https://www.parkrun.org.uk/sloughbottom/results/174/" xr:uid="{8331A748-0473-284B-9D3F-147CA024DE3E}"/>
+    <hyperlink ref="B52" r:id="rId201" display="https://www.parkrun.org.uk/catton/results/469/" xr:uid="{2CE95C8B-1FB7-8740-9AE3-AC2972D94120}"/>
+    <hyperlink ref="B51" r:id="rId202" display="https://www.parkrun.org.uk/harlestonmagpies/results/119/" xr:uid="{7CFC187C-1259-BB48-B753-8959174A7930}"/>
+    <hyperlink ref="B50" r:id="rId203" display="https://www.parkrun.org.uk/colneylane/results/249/" xr:uid="{7A8D4EE9-6DAD-C641-BABB-E020B14C8ADB}"/>
+    <hyperlink ref="B49" r:id="rId204" display="https://www.parkrun.org.uk/holkham/results/305/" xr:uid="{2946DD23-45D6-3C4A-8A1F-9A92E2F5EFF3}"/>
+    <hyperlink ref="B48" r:id="rId205" display="https://www.parkrun.org.uk/downhammarketacademy/results/92/" xr:uid="{8E4AA368-9573-2543-B992-B3899538CF99}"/>
+    <hyperlink ref="B47" r:id="rId206" display="https://www.parkrun.org.uk/sloughbottom/results/180/" xr:uid="{311FD894-FC57-F74F-A3C2-C83E6980BD86}"/>
+    <hyperlink ref="B46" r:id="rId207" display="https://www.parkrun.org.uk/brandoncountrypark/results/509/" xr:uid="{BD73B82C-6060-EC46-AF93-C0FEC7BBCBBF}"/>
+    <hyperlink ref="B45" r:id="rId208" display="https://www.parkrun.org.uk/sandringham/results/122/" xr:uid="{12A5795E-4AF7-664B-BEE8-7C9B629721F8}"/>
+    <hyperlink ref="B44" r:id="rId209" display="https://www.parkrun.org.uk/sloughbottom/results/183/" xr:uid="{A5CE83E3-6F97-6849-BB4A-CEFAA53CC597}"/>
+    <hyperlink ref="B43" r:id="rId210" display="https://www.parkrun.org.uk/gorleston/results/706/" xr:uid="{64A72A9B-DC52-204C-AF37-BAFA110BCE6A}"/>
+    <hyperlink ref="B42" r:id="rId211" display="https://www.parkrun.org.uk/sloughbottom/results/185/" xr:uid="{2139748D-B7E9-C841-BB62-6BAED97E9867}"/>
+    <hyperlink ref="B41" r:id="rId212" display="https://www.parkrun.org.uk/gorleston/results/708/" xr:uid="{0703EB07-1E70-4048-ACCF-326FA879ABD5}"/>
+    <hyperlink ref="B40" r:id="rId213" display="https://www.parkrun.org.uk/lowestoft/results/371/" xr:uid="{F8EE4D03-36D9-EF42-B22E-0B557B749314}"/>
+    <hyperlink ref="B39" r:id="rId214" display="https://www.parkrun.org.uk/swaffham/results/239/" xr:uid="{C6D9F588-E9A1-BA4C-9ACE-1EA8CD86F18A}"/>
+    <hyperlink ref="B38" r:id="rId215" display="https://www.parkrun.org.uk/sloughbottom/results/189/" xr:uid="{C83CAE3D-F6EA-A244-9339-34EE0C400C6B}"/>
+    <hyperlink ref="B37" r:id="rId216" display="https://www.parkrun.org.uk/colneylane/results/262/" xr:uid="{CADECC84-9A11-BC40-BBE9-C5932FAB9D67}"/>
+    <hyperlink ref="B36" r:id="rId217" display="https://www.parkrun.org.uk/colneylane/results/263/" xr:uid="{79D3D039-2559-A04E-8636-DECAF17F81BB}"/>
+    <hyperlink ref="B35" r:id="rId218" display="https://www.parkrun.org.uk/sloughbottom/results/192/" xr:uid="{0A93FD3D-30FC-9843-8803-4F54E7F8A3A1}"/>
+    <hyperlink ref="B34" r:id="rId219" display="https://www.parkrun.org.uk/colneylane/results/265/" xr:uid="{A73A411A-B701-2D47-92DE-A8663C135A10}"/>
+    <hyperlink ref="B33" r:id="rId220" display="https://www.parkrun.org.uk/colneylane/results/266/" xr:uid="{8816943F-8C95-1D41-9A07-38EFAEA75902}"/>
+    <hyperlink ref="B32" r:id="rId221" display="https://www.parkrun.org.uk/colneylane/results/267/" xr:uid="{07710C45-F599-1E4D-93E6-F90C7403BBFA}"/>
+    <hyperlink ref="B31" r:id="rId222" display="https://www.parkrun.org.uk/sloughbottom/results/196/" xr:uid="{53E33B80-772A-994D-B8CC-81F4B5E1216C}"/>
+    <hyperlink ref="B30" r:id="rId223" display="https://www.parkrun.org.uk/greatyarmouthnorthbeach/results/152/" xr:uid="{2730402E-D4EF-3B42-8108-749F9C50DBB7}"/>
+    <hyperlink ref="B29" r:id="rId224" display="https://www.parkrun.org.uk/colneylane/results/270/" xr:uid="{E9F2661D-A713-184F-B7D4-2C2E0C4921C8}"/>
+    <hyperlink ref="B28" r:id="rId225" display="https://www.parkrun.org.uk/catton/results/493/" xr:uid="{D6A6D1BB-92BF-C042-B713-DFB2774AA23B}"/>
+    <hyperlink ref="B27" r:id="rId226" display="https://www.parkrun.org.uk/sloughbottom/results/200/" xr:uid="{8338BA8E-B390-DD47-86A2-BC0AC0DE01D4}"/>
+    <hyperlink ref="B26" r:id="rId227" display="https://www.parkrun.org.uk/colneylane/results/273/" xr:uid="{C30BC857-AC17-4F41-BC60-EAA6D83AC68C}"/>
+    <hyperlink ref="B25" r:id="rId228" display="https://www.parkrun.org.uk/colneylane/results/274/" xr:uid="{ADCF8407-F39F-644A-A2D5-5C37714E0B34}"/>
+    <hyperlink ref="B24" r:id="rId229" display="https://www.parkrun.org.uk/sloughbottom/results/203/" xr:uid="{904D2D68-EC1F-ED4A-86A2-98004ABCD0E5}"/>
+    <hyperlink ref="B23" r:id="rId230" display="https://www.parkrun.org.uk/sloughbottom/results/204/" xr:uid="{2758B14F-ECAD-A149-B9CA-DCDDBF51F853}"/>
+    <hyperlink ref="B22" r:id="rId231" display="https://www.parkrun.org.uk/lancingbeachgreen/results/214/" xr:uid="{79550B87-89E2-7041-A9E1-B0215D44BCEB}"/>
+    <hyperlink ref="B21" r:id="rId232" display="https://www.parkrun.org.uk/sharphamroadplayingfields/results/142/" xr:uid="{8099819A-DCE9-574A-BE0F-42661BEF8E16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>